<commit_message>
✨ Item-item CF: complete part 3
</commit_message>
<xml_diff>
--- a/recommender-systems/collaborative-filtering/Assignment 5.xlsx
+++ b/recommender-systems/collaborative-filtering/Assignment 5.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eigenein/GitHub/coursera/recommender-systems/collaborative-filtering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A944EB65-F9FD-A749-8A53-1D2BEC46DF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB560C1-6EE3-A64C-B47A-B7790D246637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratings" sheetId="1" r:id="rId1"/>
     <sheet name="NormRatings" sheetId="5" r:id="rId2"/>
     <sheet name="Matrix" sheetId="4" r:id="rId3"/>
     <sheet name="FilterMatrix" sheetId="6" r:id="rId4"/>
+    <sheet name="NormMatrix" sheetId="7" r:id="rId5"/>
+    <sheet name="NormFilterMatrix" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="29">
   <si>
     <t>User</t>
   </si>
@@ -961,11 +963,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4016,7 +4018,7 @@
   <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
@@ -5883,7 +5885,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C21"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7773,4 +7775,3758 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E999292-929F-5D44-A9C4-CEFC5E49125E}">
+  <dimension ref="A1:U44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!B$2:B$21) / NormRatings!$B$22 / NormRatings!B$22</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!C$2:C$21) / NormRatings!$B$22 / NormRatings!C$22</f>
+        <v>-0.3777707025577885</v>
+      </c>
+      <c r="D2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!D$2:D$21) / NormRatings!$B$22 / NormRatings!D$22</f>
+        <v>0.35577972454766571</v>
+      </c>
+      <c r="E2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!E$2:E$21) / NormRatings!$B$22 / NormRatings!E$22</f>
+        <v>0.21597537370665254</v>
+      </c>
+      <c r="F2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!F$2:F$21) / NormRatings!$B$22 / NormRatings!F$22</f>
+        <v>-0.60370783052315868</v>
+      </c>
+      <c r="G2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!G$2:G$21) / NormRatings!$B$22 / NormRatings!G$22</f>
+        <v>0.13921371111490649</v>
+      </c>
+      <c r="H2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!H$2:H$21) / NormRatings!$B$22 / NormRatings!H$22</f>
+        <v>-5.0337551330349603E-2</v>
+      </c>
+      <c r="I2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!I$2:I$21) / NormRatings!$B$22 / NormRatings!I$22</f>
+        <v>0.19279858482944665</v>
+      </c>
+      <c r="J2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!J$2:J$21) / NormRatings!$B$22 / NormRatings!J$22</f>
+        <v>0.29501316508704811</v>
+      </c>
+      <c r="K2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!K$2:K$21) / NormRatings!$B$22 / NormRatings!K$22</f>
+        <v>-0.22565691806008556</v>
+      </c>
+      <c r="L2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!L$2:L$21) / NormRatings!$B$22 / NormRatings!L$22</f>
+        <v>0.11675543916439571</v>
+      </c>
+      <c r="M2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!M$2:M$21) / NormRatings!$B$22 / NormRatings!M$22</f>
+        <v>0.18471220265778823</v>
+      </c>
+      <c r="N2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!N$2:N$21) / NormRatings!$B$22 / NormRatings!N$22</f>
+        <v>-0.31990411258573898</v>
+      </c>
+      <c r="O2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!O$2:O$21) / NormRatings!$B$22 / NormRatings!O$22</f>
+        <v>2.0007385508959367E-2</v>
+      </c>
+      <c r="P2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!P$2:P$21) / NormRatings!$B$22 / NormRatings!P$22</f>
+        <v>-0.10558369236125581</v>
+      </c>
+      <c r="Q2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!Q$2:Q$21) / NormRatings!$B$22 / NormRatings!Q$22</f>
+        <v>-0.42033136932878529</v>
+      </c>
+      <c r="R2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!R$2:R$21) / NormRatings!$B$22 / NormRatings!R$22</f>
+        <v>-0.1467836107802884</v>
+      </c>
+      <c r="S2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!S$2:S$21) / NormRatings!$B$22 / NormRatings!S$22</f>
+        <v>-0.24128093854653215</v>
+      </c>
+      <c r="T2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!T$2:T$21) / NormRatings!$B$22 / NormRatings!T$22</f>
+        <v>-0.24885679814496334</v>
+      </c>
+      <c r="U2">
+        <f>SUMPRODUCT(NormRatings!$B$2:$B$21, NormRatings!U$2:U$21) / NormRatings!$B$22 / NormRatings!U$22</f>
+        <v>0.55444750193353987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!B$2:B$21) / NormRatings!$C$22 / NormRatings!B$22</f>
+        <v>-0.3777707025577885</v>
+      </c>
+      <c r="C3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!C$2:C$21) / NormRatings!$C$22 / NormRatings!C$22</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="D3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!D$2:D$21) / NormRatings!$C$22 / NormRatings!D$22</f>
+        <v>-0.50403807526446875</v>
+      </c>
+      <c r="E3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!E$2:E$21) / NormRatings!$C$22 / NormRatings!E$22</f>
+        <v>3.5870569165431928E-3</v>
+      </c>
+      <c r="F3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!F$2:F$21) / NormRatings!$C$22 / NormRatings!F$22</f>
+        <v>-2.3219011917351404E-2</v>
+      </c>
+      <c r="G3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!G$2:G$21) / NormRatings!$C$22 / NormRatings!G$22</f>
+        <v>-0.32870333645184219</v>
+      </c>
+      <c r="H3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!H$2:H$21) / NormRatings!$C$22 / NormRatings!H$22</f>
+        <v>-0.23149600029916106</v>
+      </c>
+      <c r="I3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!I$2:I$21) / NormRatings!$C$22 / NormRatings!I$22</f>
+        <v>-0.15633194923970942</v>
+      </c>
+      <c r="J3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!J$2:J$21) / NormRatings!$C$22 / NormRatings!J$22</f>
+        <v>1.3543190284680795E-2</v>
+      </c>
+      <c r="K3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!K$2:K$21) / NormRatings!$C$22 / NormRatings!K$22</f>
+        <v>0.31518507647562766</v>
+      </c>
+      <c r="L3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!L$2:L$21) / NormRatings!$C$22 / NormRatings!L$22</f>
+        <v>0.15540846526009983</v>
+      </c>
+      <c r="M3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!M$2:M$21) / NormRatings!$C$22 / NormRatings!M$22</f>
+        <v>-3.6622272121207217E-3</v>
+      </c>
+      <c r="N3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!N$2:N$21) / NormRatings!$C$22 / NormRatings!N$22</f>
+        <v>0.49391225217014639</v>
+      </c>
+      <c r="O3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!O$2:O$21) / NormRatings!$C$22 / NormRatings!O$22</f>
+        <v>-0.15988213159788864</v>
+      </c>
+      <c r="P3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!P$2:P$21) / NormRatings!$C$22 / NormRatings!P$22</f>
+        <v>-0.27148913396548996</v>
+      </c>
+      <c r="Q3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!Q$2:Q$21) / NormRatings!$C$22 / NormRatings!Q$22</f>
+        <v>0.43588474936768895</v>
+      </c>
+      <c r="R3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!R$2:R$21) / NormRatings!$C$22 / NormRatings!R$22</f>
+        <v>-0.25027372858887026</v>
+      </c>
+      <c r="S3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!S$2:S$21) / NormRatings!$C$22 / NormRatings!S$22</f>
+        <v>1.6440895757123954E-2</v>
+      </c>
+      <c r="T3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!T$2:T$21) / NormRatings!$C$22 / NormRatings!T$22</f>
+        <v>3.8345942402239333E-2</v>
+      </c>
+      <c r="U3">
+        <f>SUMPRODUCT(NormRatings!$C$2:$C$21, NormRatings!U$2:U$21) / NormRatings!$C$22 / NormRatings!U$22</f>
+        <v>-0.32287453355402218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!B$2:B$21) / NormRatings!$D$22 / NormRatings!B$22</f>
+        <v>0.35577972454766577</v>
+      </c>
+      <c r="C4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!C$2:C$21) / NormRatings!$D$22 / NormRatings!C$22</f>
+        <v>-0.50403807526446875</v>
+      </c>
+      <c r="D4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!D$2:D$21) / NormRatings!$D$22 / NormRatings!D$22</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!E$2:E$21) / NormRatings!$D$22 / NormRatings!E$22</f>
+        <v>-0.30523200487726299</v>
+      </c>
+      <c r="F4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!F$2:F$21) / NormRatings!$D$22 / NormRatings!F$22</f>
+        <v>2.3469953903822744E-2</v>
+      </c>
+      <c r="G4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!G$2:G$21) / NormRatings!$D$22 / NormRatings!G$22</f>
+        <v>0.39156391871191337</v>
+      </c>
+      <c r="H4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!H$2:H$21) / NormRatings!$D$22 / NormRatings!H$22</f>
+        <v>0.10094588826430767</v>
+      </c>
+      <c r="I4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!I$2:I$21) / NormRatings!$D$22 / NormRatings!I$22</f>
+        <v>7.5201233799563505E-2</v>
+      </c>
+      <c r="J4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!J$2:J$21) / NormRatings!$D$22 / NormRatings!J$22</f>
+        <v>-3.1831782474374931E-2</v>
+      </c>
+      <c r="K4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!K$2:K$21) / NormRatings!$D$22 / NormRatings!K$22</f>
+        <v>0.1940588267347674</v>
+      </c>
+      <c r="L4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!L$2:L$21) / NormRatings!$D$22 / NormRatings!L$22</f>
+        <v>0.13382387317628316</v>
+      </c>
+      <c r="M4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!M$2:M$21) / NormRatings!$D$22 / NormRatings!M$22</f>
+        <v>-0.18423079907615575</v>
+      </c>
+      <c r="N4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!N$2:N$21) / NormRatings!$D$22 / NormRatings!N$22</f>
+        <v>-0.19900110135419802</v>
+      </c>
+      <c r="O4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!O$2:O$21) / NormRatings!$D$22 / NormRatings!O$22</f>
+        <v>-0.15886032348178078</v>
+      </c>
+      <c r="P4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!P$2:P$21) / NormRatings!$D$22 / NormRatings!P$22</f>
+        <v>-0.25831232083260147</v>
+      </c>
+      <c r="Q4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!Q$2:Q$21) / NormRatings!$D$22 / NormRatings!Q$22</f>
+        <v>-0.34446330285480997</v>
+      </c>
+      <c r="R4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!R$2:R$21) / NormRatings!$D$22 / NormRatings!R$22</f>
+        <v>0.27157977147770279</v>
+      </c>
+      <c r="S4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!S$2:S$21) / NormRatings!$D$22 / NormRatings!S$22</f>
+        <v>-0.12000690061044302</v>
+      </c>
+      <c r="T4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!T$2:T$21) / NormRatings!$D$22 / NormRatings!T$22</f>
+        <v>-7.649363964232464E-2</v>
+      </c>
+      <c r="U4">
+        <f>SUMPRODUCT(NormRatings!$D$2:$D$21, NormRatings!U$2:U$21) / NormRatings!$D$22 / NormRatings!U$22</f>
+        <v>-0.24015520716514135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!B$2:B$21) / NormRatings!$E$22 / NormRatings!B$22</f>
+        <v>0.21597537370665254</v>
+      </c>
+      <c r="C5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!C$2:C$21) / NormRatings!$E$22 / NormRatings!C$22</f>
+        <v>3.5870569165431928E-3</v>
+      </c>
+      <c r="D5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!D$2:D$21) / NormRatings!$E$22 / NormRatings!D$22</f>
+        <v>-0.30523200487726304</v>
+      </c>
+      <c r="E5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!E$2:E$21) / NormRatings!$E$22 / NormRatings!E$22</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!F$2:F$21) / NormRatings!$E$22 / NormRatings!F$22</f>
+        <v>-0.18619213695287481</v>
+      </c>
+      <c r="G5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!G$2:G$21) / NormRatings!$E$22 / NormRatings!G$22</f>
+        <v>-1.0114150886013135E-3</v>
+      </c>
+      <c r="H5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!H$2:H$21) / NormRatings!$E$22 / NormRatings!H$22</f>
+        <v>-0.1948690490083354</v>
+      </c>
+      <c r="I5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!I$2:I$21) / NormRatings!$E$22 / NormRatings!I$22</f>
+        <v>-0.27641254856047098</v>
+      </c>
+      <c r="J5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!J$2:J$21) / NormRatings!$E$22 / NormRatings!J$22</f>
+        <v>0.34361515261779119</v>
+      </c>
+      <c r="K5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!K$2:K$21) / NormRatings!$E$22 / NormRatings!K$22</f>
+        <v>-6.2223812290357304E-2</v>
+      </c>
+      <c r="L5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!L$2:L$21) / NormRatings!$E$22 / NormRatings!L$22</f>
+        <v>-9.6726647455324846E-2</v>
+      </c>
+      <c r="M5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!M$2:M$21) / NormRatings!$E$22 / NormRatings!M$22</f>
+        <v>-4.9894481494938074E-2</v>
+      </c>
+      <c r="N5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!N$2:N$21) / NormRatings!$E$22 / NormRatings!N$22</f>
+        <v>0.13502180347281489</v>
+      </c>
+      <c r="O5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!O$2:O$21) / NormRatings!$E$22 / NormRatings!O$22</f>
+        <v>0.34122912118567683</v>
+      </c>
+      <c r="P5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!P$2:P$21) / NormRatings!$E$22 / NormRatings!P$22</f>
+        <v>-0.1012842614062975</v>
+      </c>
+      <c r="Q5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!Q$2:Q$21) / NormRatings!$E$22 / NormRatings!Q$22</f>
+        <v>-6.7329350700858354E-2</v>
+      </c>
+      <c r="R5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!R$2:R$21) / NormRatings!$E$22 / NormRatings!R$22</f>
+        <v>-0.21326361555047879</v>
+      </c>
+      <c r="S5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!S$2:S$21) / NormRatings!$E$22 / NormRatings!S$22</f>
+        <v>-0.26148228822764069</v>
+      </c>
+      <c r="T5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!T$2:T$21) / NormRatings!$E$22 / NormRatings!T$22</f>
+        <v>-0.34376595143984073</v>
+      </c>
+      <c r="U5">
+        <f>SUMPRODUCT(NormRatings!$E$2:$E$21, NormRatings!U$2:U$21) / NormRatings!$E$22 / NormRatings!U$22</f>
+        <v>0.32353240190383042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!B$2:B$21) / NormRatings!$F$22 / NormRatings!B$22</f>
+        <v>-0.60370783052315868</v>
+      </c>
+      <c r="C6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!C$2:C$21) / NormRatings!$F$22 / NormRatings!C$22</f>
+        <v>-2.3219011917351401E-2</v>
+      </c>
+      <c r="D6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!D$2:D$21) / NormRatings!$F$22 / NormRatings!D$22</f>
+        <v>2.3469953903822744E-2</v>
+      </c>
+      <c r="E6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!E$2:E$21) / NormRatings!$F$22 / NormRatings!E$22</f>
+        <v>-0.18619213695287481</v>
+      </c>
+      <c r="F6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!F$2:F$21) / NormRatings!$F$22 / NormRatings!F$22</f>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!G$2:G$21) / NormRatings!$F$22 / NormRatings!G$22</f>
+        <v>8.8281840279244864E-2</v>
+      </c>
+      <c r="H6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!H$2:H$21) / NormRatings!$F$22 / NormRatings!H$22</f>
+        <v>-0.28667003262351204</v>
+      </c>
+      <c r="I6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!I$2:I$21) / NormRatings!$F$22 / NormRatings!I$22</f>
+        <v>-0.29988267181483513</v>
+      </c>
+      <c r="J6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!J$2:J$21) / NormRatings!$F$22 / NormRatings!J$22</f>
+        <v>-0.34655862561821971</v>
+      </c>
+      <c r="K6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!K$2:K$21) / NormRatings!$F$22 / NormRatings!K$22</f>
+        <v>0.11286299690121732</v>
+      </c>
+      <c r="L6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!L$2:L$21) / NormRatings!$F$22 / NormRatings!L$22</f>
+        <v>8.9045163112599843E-2</v>
+      </c>
+      <c r="M6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!M$2:M$21) / NormRatings!$F$22 / NormRatings!M$22</f>
+        <v>-0.27600320586083976</v>
+      </c>
+      <c r="N6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!N$2:N$21) / NormRatings!$F$22 / NormRatings!N$22</f>
+        <v>0.19636854834003448</v>
+      </c>
+      <c r="O6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!O$2:O$21) / NormRatings!$F$22 / NormRatings!O$22</f>
+        <v>2.5442197927654141E-2</v>
+      </c>
+      <c r="P6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!P$2:P$21) / NormRatings!$F$22 / NormRatings!P$22</f>
+        <v>1.1303188058154643E-2</v>
+      </c>
+      <c r="Q6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!Q$2:Q$21) / NormRatings!$F$22 / NormRatings!Q$22</f>
+        <v>0.1803656901652074</v>
+      </c>
+      <c r="R6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!R$2:R$21) / NormRatings!$F$22 / NormRatings!R$22</f>
+        <v>0.2277775932481598</v>
+      </c>
+      <c r="S6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!S$2:S$21) / NormRatings!$F$22 / NormRatings!S$22</f>
+        <v>0.40132014193944721</v>
+      </c>
+      <c r="T6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!T$2:T$21) / NormRatings!$F$22 / NormRatings!T$22</f>
+        <v>-1.0013615857306585E-2</v>
+      </c>
+      <c r="U6">
+        <f>SUMPRODUCT(NormRatings!$F$2:$F$21, NormRatings!U$2:U$21) / NormRatings!$F$22 / NormRatings!U$22</f>
+        <v>-0.45992867072689786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!B$2:B$21) / NormRatings!$G$22 / NormRatings!B$22</f>
+        <v>0.13921371111490652</v>
+      </c>
+      <c r="C7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!C$2:C$21) / NormRatings!$G$22 / NormRatings!C$22</f>
+        <v>-0.32870333645184219</v>
+      </c>
+      <c r="D7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!D$2:D$21) / NormRatings!$G$22 / NormRatings!D$22</f>
+        <v>0.39156391871191343</v>
+      </c>
+      <c r="E7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!E$2:E$21) / NormRatings!$G$22 / NormRatings!E$22</f>
+        <v>-1.0114150886013135E-3</v>
+      </c>
+      <c r="F7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!F$2:F$21) / NormRatings!$G$22 / NormRatings!F$22</f>
+        <v>8.8281840279244864E-2</v>
+      </c>
+      <c r="G7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!G$2:G$21) / NormRatings!$G$22 / NormRatings!G$22</f>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!H$2:H$21) / NormRatings!$G$22 / NormRatings!H$22</f>
+        <v>-4.4092056266285505E-2</v>
+      </c>
+      <c r="I7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!I$2:I$21) / NormRatings!$G$22 / NormRatings!I$22</f>
+        <v>-5.1687923562043978E-2</v>
+      </c>
+      <c r="J7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!J$2:J$21) / NormRatings!$G$22 / NormRatings!J$22</f>
+        <v>-0.37423359160676045</v>
+      </c>
+      <c r="K7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!K$2:K$21) / NormRatings!$G$22 / NormRatings!K$22</f>
+        <v>0.27830998560508052</v>
+      </c>
+      <c r="L7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!L$2:L$21) / NormRatings!$G$22 / NormRatings!L$22</f>
+        <v>-0.35593698229136417</v>
+      </c>
+      <c r="M7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!M$2:M$21) / NormRatings!$G$22 / NormRatings!M$22</f>
+        <v>-8.0608567092191788E-2</v>
+      </c>
+      <c r="N7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!N$2:N$21) / NormRatings!$G$22 / NormRatings!N$22</f>
+        <v>-1.7288710808306108E-2</v>
+      </c>
+      <c r="O7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!O$2:O$21) / NormRatings!$G$22 / NormRatings!O$22</f>
+        <v>-0.24127474155355685</v>
+      </c>
+      <c r="P7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!P$2:P$21) / NormRatings!$G$22 / NormRatings!P$22</f>
+        <v>-0.12845327480426177</v>
+      </c>
+      <c r="Q7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!Q$2:Q$21) / NormRatings!$G$22 / NormRatings!Q$22</f>
+        <v>-0.21773793467394631</v>
+      </c>
+      <c r="R7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!R$2:R$21) / NormRatings!$G$22 / NormRatings!R$22</f>
+        <v>-0.27689129094030845</v>
+      </c>
+      <c r="S7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!S$2:S$21) / NormRatings!$G$22 / NormRatings!S$22</f>
+        <v>0.1314578096042659</v>
+      </c>
+      <c r="T7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!T$2:T$21) / NormRatings!$G$22 / NormRatings!T$22</f>
+        <v>0.10060165349150764</v>
+      </c>
+      <c r="U7">
+        <f>SUMPRODUCT(NormRatings!$G$2:$G$21, NormRatings!U$2:U$21) / NormRatings!$G$22 / NormRatings!U$22</f>
+        <v>-0.18024862598365846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!B$2:B$21) / NormRatings!$H$22 / NormRatings!B$22</f>
+        <v>-5.0337551330349596E-2</v>
+      </c>
+      <c r="C8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!C$2:C$21) / NormRatings!$H$22 / NormRatings!C$22</f>
+        <v>-0.23149600029916106</v>
+      </c>
+      <c r="D8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!D$2:D$21) / NormRatings!$H$22 / NormRatings!D$22</f>
+        <v>0.10094588826430768</v>
+      </c>
+      <c r="E8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!E$2:E$21) / NormRatings!$H$22 / NormRatings!E$22</f>
+        <v>-0.1948690490083354</v>
+      </c>
+      <c r="F8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!F$2:F$21) / NormRatings!$H$22 / NormRatings!F$22</f>
+        <v>-0.28667003262351209</v>
+      </c>
+      <c r="G8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!G$2:G$21) / NormRatings!$H$22 / NormRatings!G$22</f>
+        <v>-4.4092056266285512E-2</v>
+      </c>
+      <c r="H8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!H$2:H$21) / NormRatings!$H$22 / NormRatings!H$22</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!I$2:I$21) / NormRatings!$H$22 / NormRatings!I$22</f>
+        <v>0.17472391669004284</v>
+      </c>
+      <c r="J8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!J$2:J$21) / NormRatings!$H$22 / NormRatings!J$22</f>
+        <v>0.19190832656287304</v>
+      </c>
+      <c r="K8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!K$2:K$21) / NormRatings!$H$22 / NormRatings!K$22</f>
+        <v>7.0879871588571536E-2</v>
+      </c>
+      <c r="L8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!L$2:L$21) / NormRatings!$H$22 / NormRatings!L$22</f>
+        <v>0.1308552371719458</v>
+      </c>
+      <c r="M8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!M$2:M$21) / NormRatings!$H$22 / NormRatings!M$22</f>
+        <v>-0.22402664855014137</v>
+      </c>
+      <c r="N8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!N$2:N$21) / NormRatings!$H$22 / NormRatings!N$22</f>
+        <v>-0.61244883080582968</v>
+      </c>
+      <c r="O8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!O$2:O$21) / NormRatings!$H$22 / NormRatings!O$22</f>
+        <v>-2.9116748707301895E-2</v>
+      </c>
+      <c r="P8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!P$2:P$21) / NormRatings!$H$22 / NormRatings!P$22</f>
+        <v>-6.3479295498554841E-2</v>
+      </c>
+      <c r="Q8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!Q$2:Q$21) / NormRatings!$H$22 / NormRatings!Q$22</f>
+        <v>-0.19215041457752635</v>
+      </c>
+      <c r="R8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!R$2:R$21) / NormRatings!$H$22 / NormRatings!R$22</f>
+        <v>0.23091237747387072</v>
+      </c>
+      <c r="S8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!S$2:S$21) / NormRatings!$H$22 / NormRatings!S$22</f>
+        <v>-0.40826013627367458</v>
+      </c>
+      <c r="T8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!T$2:T$21) / NormRatings!$H$22 / NormRatings!T$22</f>
+        <v>0.18484479215240943</v>
+      </c>
+      <c r="U8">
+        <f>SUMPRODUCT(NormRatings!$H$2:$H$21, NormRatings!U$2:U$21) / NormRatings!$H$22 / NormRatings!U$22</f>
+        <v>9.585275771229157E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!B$2:B$21) / NormRatings!$I$22 / NormRatings!B$22</f>
+        <v>0.19279858482944665</v>
+      </c>
+      <c r="C9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!C$2:C$21) / NormRatings!$I$22 / NormRatings!C$22</f>
+        <v>-0.15633194923970942</v>
+      </c>
+      <c r="D9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!D$2:D$21) / NormRatings!$I$22 / NormRatings!D$22</f>
+        <v>7.5201233799563519E-2</v>
+      </c>
+      <c r="E9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!E$2:E$21) / NormRatings!$I$22 / NormRatings!E$22</f>
+        <v>-0.27641254856047098</v>
+      </c>
+      <c r="F9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!F$2:F$21) / NormRatings!$I$22 / NormRatings!F$22</f>
+        <v>-0.29988267181483513</v>
+      </c>
+      <c r="G9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!G$2:G$21) / NormRatings!$I$22 / NormRatings!G$22</f>
+        <v>-5.1687923562043978E-2</v>
+      </c>
+      <c r="H9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!H$2:H$21) / NormRatings!$I$22 / NormRatings!H$22</f>
+        <v>0.17472391669004284</v>
+      </c>
+      <c r="I9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!I$2:I$21) / NormRatings!$I$22 / NormRatings!I$22</f>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!J$2:J$21) / NormRatings!$I$22 / NormRatings!J$22</f>
+        <v>-0.27857527950646432</v>
+      </c>
+      <c r="K9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!K$2:K$21) / NormRatings!$I$22 / NormRatings!K$22</f>
+        <v>-0.2480569510013424</v>
+      </c>
+      <c r="L9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!L$2:L$21) / NormRatings!$I$22 / NormRatings!L$22</f>
+        <v>-0.39609918584700499</v>
+      </c>
+      <c r="M9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!M$2:M$21) / NormRatings!$I$22 / NormRatings!M$22</f>
+        <v>4.5156230400746289E-2</v>
+      </c>
+      <c r="N9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!N$2:N$21) / NormRatings!$I$22 / NormRatings!N$22</f>
+        <v>-0.29114935032904599</v>
+      </c>
+      <c r="O9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!O$2:O$21) / NormRatings!$I$22 / NormRatings!O$22</f>
+        <v>0.20169374985070956</v>
+      </c>
+      <c r="P9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!P$2:P$21) / NormRatings!$I$22 / NormRatings!P$22</f>
+        <v>0.13606351293652716</v>
+      </c>
+      <c r="Q9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!Q$2:Q$21) / NormRatings!$I$22 / NormRatings!Q$22</f>
+        <v>-0.18719824061676185</v>
+      </c>
+      <c r="R9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!R$2:R$21) / NormRatings!$I$22 / NormRatings!R$22</f>
+        <v>0.15849371661451467</v>
+      </c>
+      <c r="S9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!S$2:S$21) / NormRatings!$I$22 / NormRatings!S$22</f>
+        <v>-7.1244359962643722E-2</v>
+      </c>
+      <c r="T9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!T$2:T$21) / NormRatings!$I$22 / NormRatings!T$22</f>
+        <v>0.331349590586206</v>
+      </c>
+      <c r="U9">
+        <f>SUMPRODUCT(NormRatings!$I$2:$I$21, NormRatings!U$2:U$21) / NormRatings!$I$22 / NormRatings!U$22</f>
+        <v>6.9644128532871608E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!B$2:B$21) / NormRatings!$J$22 / NormRatings!B$22</f>
+        <v>0.29501316508704806</v>
+      </c>
+      <c r="C10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!C$2:C$21) / NormRatings!$J$22 / NormRatings!C$22</f>
+        <v>1.3543190284680796E-2</v>
+      </c>
+      <c r="D10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!D$2:D$21) / NormRatings!$J$22 / NormRatings!D$22</f>
+        <v>-3.1831782474374931E-2</v>
+      </c>
+      <c r="E10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!E$2:E$21) / NormRatings!$J$22 / NormRatings!E$22</f>
+        <v>0.34361515261779119</v>
+      </c>
+      <c r="F10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!F$2:F$21) / NormRatings!$J$22 / NormRatings!F$22</f>
+        <v>-0.34655862561821971</v>
+      </c>
+      <c r="G10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!G$2:G$21) / NormRatings!$J$22 / NormRatings!G$22</f>
+        <v>-0.37423359160676045</v>
+      </c>
+      <c r="H10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!H$2:H$21) / NormRatings!$J$22 / NormRatings!H$22</f>
+        <v>0.19190832656287307</v>
+      </c>
+      <c r="I10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!I$2:I$21) / NormRatings!$J$22 / NormRatings!I$22</f>
+        <v>-0.27857527950646438</v>
+      </c>
+      <c r="J10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!J$2:J$21) / NormRatings!$J$22 / NormRatings!J$22</f>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!K$2:K$21) / NormRatings!$J$22 / NormRatings!K$22</f>
+        <v>0.12081715289101295</v>
+      </c>
+      <c r="L10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!L$2:L$21) / NormRatings!$J$22 / NormRatings!L$22</f>
+        <v>0.32648908513771746</v>
+      </c>
+      <c r="M10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!M$2:M$21) / NormRatings!$J$22 / NormRatings!M$22</f>
+        <v>-1.3461527896611125E-2</v>
+      </c>
+      <c r="N10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!N$2:N$21) / NormRatings!$J$22 / NormRatings!N$22</f>
+        <v>-0.14510149809175907</v>
+      </c>
+      <c r="O10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!O$2:O$21) / NormRatings!$J$22 / NormRatings!O$22</f>
+        <v>-5.1592564238564662E-2</v>
+      </c>
+      <c r="P10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!P$2:P$21) / NormRatings!$J$22 / NormRatings!P$22</f>
+        <v>1.8982634310231183E-2</v>
+      </c>
+      <c r="Q10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!Q$2:Q$21) / NormRatings!$J$22 / NormRatings!Q$22</f>
+        <v>-0.3486830932414996</v>
+      </c>
+      <c r="R10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!R$2:R$21) / NormRatings!$J$22 / NormRatings!R$22</f>
+        <v>8.8526348280390341E-2</v>
+      </c>
+      <c r="S10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!S$2:S$21) / NormRatings!$J$22 / NormRatings!S$22</f>
+        <v>-0.53011055804302232</v>
+      </c>
+      <c r="T10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!T$2:T$21) / NormRatings!$J$22 / NormRatings!T$22</f>
+        <v>-0.2919826131803987</v>
+      </c>
+      <c r="U10">
+        <f>SUMPRODUCT(NormRatings!$J$2:$J$21, NormRatings!U$2:U$21) / NormRatings!$J$22 / NormRatings!U$22</f>
+        <v>0.26172689797317195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!B$2:B$21) / NormRatings!$K$22 / NormRatings!B$22</f>
+        <v>-0.22565691806008559</v>
+      </c>
+      <c r="C11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!C$2:C$21) / NormRatings!$K$22 / NormRatings!C$22</f>
+        <v>0.31518507647562766</v>
+      </c>
+      <c r="D11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!D$2:D$21) / NormRatings!$K$22 / NormRatings!D$22</f>
+        <v>0.19405882673476738</v>
+      </c>
+      <c r="E11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!E$2:E$21) / NormRatings!$K$22 / NormRatings!E$22</f>
+        <v>-6.2223812290357311E-2</v>
+      </c>
+      <c r="F11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!F$2:F$21) / NormRatings!$K$22 / NormRatings!F$22</f>
+        <v>0.11286299690121732</v>
+      </c>
+      <c r="G11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!G$2:G$21) / NormRatings!$K$22 / NormRatings!G$22</f>
+        <v>0.27830998560508052</v>
+      </c>
+      <c r="H11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!H$2:H$21) / NormRatings!$K$22 / NormRatings!H$22</f>
+        <v>7.0879871588571536E-2</v>
+      </c>
+      <c r="I11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!I$2:I$21) / NormRatings!$K$22 / NormRatings!I$22</f>
+        <v>-0.2480569510013424</v>
+      </c>
+      <c r="J11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!J$2:J$21) / NormRatings!$K$22 / NormRatings!J$22</f>
+        <v>0.12081715289101294</v>
+      </c>
+      <c r="K11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!K$2:K$21) / NormRatings!$K$22 / NormRatings!K$22</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="L11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!L$2:L$21) / NormRatings!$K$22 / NormRatings!L$22</f>
+        <v>-1.5650146115978675E-2</v>
+      </c>
+      <c r="M11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!M$2:M$21) / NormRatings!$K$22 / NormRatings!M$22</f>
+        <v>-9.4090523296631742E-2</v>
+      </c>
+      <c r="N11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!N$2:N$21) / NormRatings!$K$22 / NormRatings!N$22</f>
+        <v>3.9140065910084794E-2</v>
+      </c>
+      <c r="O11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!O$2:O$21) / NormRatings!$K$22 / NormRatings!O$22</f>
+        <v>-0.43639678659297193</v>
+      </c>
+      <c r="P11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!P$2:P$21) / NormRatings!$K$22 / NormRatings!P$22</f>
+        <v>-0.37381482374619707</v>
+      </c>
+      <c r="Q11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!Q$2:Q$21) / NormRatings!$K$22 / NormRatings!Q$22</f>
+        <v>0.21487516831849043</v>
+      </c>
+      <c r="R11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!R$2:R$21) / NormRatings!$K$22 / NormRatings!R$22</f>
+        <v>-8.3199272055368576E-2</v>
+      </c>
+      <c r="S11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!S$2:S$21) / NormRatings!$K$22 / NormRatings!S$22</f>
+        <v>-0.45821341144447997</v>
+      </c>
+      <c r="T11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!T$2:T$21) / NormRatings!$K$22 / NormRatings!T$22</f>
+        <v>5.520677315653464E-2</v>
+      </c>
+      <c r="U11">
+        <f>SUMPRODUCT(NormRatings!$K$2:$K$21, NormRatings!U$2:U$21) / NormRatings!$K$22 / NormRatings!U$22</f>
+        <v>-0.58553091006906921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!B$2:B$21) / NormRatings!$L$22 / NormRatings!B$22</f>
+        <v>0.11675543916439569</v>
+      </c>
+      <c r="C12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!C$2:C$21) / NormRatings!$L$22 / NormRatings!C$22</f>
+        <v>0.15540846526009983</v>
+      </c>
+      <c r="D12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!D$2:D$21) / NormRatings!$L$22 / NormRatings!D$22</f>
+        <v>0.13382387317628316</v>
+      </c>
+      <c r="E12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!E$2:E$21) / NormRatings!$L$22 / NormRatings!E$22</f>
+        <v>-9.6726647455324846E-2</v>
+      </c>
+      <c r="F12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!F$2:F$21) / NormRatings!$L$22 / NormRatings!F$22</f>
+        <v>8.9045163112599843E-2</v>
+      </c>
+      <c r="G12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!G$2:G$21) / NormRatings!$L$22 / NormRatings!G$22</f>
+        <v>-0.35593698229136417</v>
+      </c>
+      <c r="H12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!H$2:H$21) / NormRatings!$L$22 / NormRatings!H$22</f>
+        <v>0.1308552371719458</v>
+      </c>
+      <c r="I12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!I$2:I$21) / NormRatings!$L$22 / NormRatings!I$22</f>
+        <v>-0.39609918584700499</v>
+      </c>
+      <c r="J12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!J$2:J$21) / NormRatings!$L$22 / NormRatings!J$22</f>
+        <v>0.32648908513771746</v>
+      </c>
+      <c r="K12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!K$2:K$21) / NormRatings!$L$22 / NormRatings!K$22</f>
+        <v>-1.5650146115978675E-2</v>
+      </c>
+      <c r="L12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!L$2:L$21) / NormRatings!$L$22 / NormRatings!L$22</f>
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!M$2:M$21) / NormRatings!$L$22 / NormRatings!M$22</f>
+        <v>-0.29565422923782619</v>
+      </c>
+      <c r="N12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!N$2:N$21) / NormRatings!$L$22 / NormRatings!N$22</f>
+        <v>-7.0377526347472519E-2</v>
+      </c>
+      <c r="O12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!O$2:O$21) / NormRatings!$L$22 / NormRatings!O$22</f>
+        <v>-0.10948502043464493</v>
+      </c>
+      <c r="P12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!P$2:P$21) / NormRatings!$L$22 / NormRatings!P$22</f>
+        <v>-0.51785889843625921</v>
+      </c>
+      <c r="Q12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!Q$2:Q$21) / NormRatings!$L$22 / NormRatings!Q$22</f>
+        <v>-0.10780486878852016</v>
+      </c>
+      <c r="R12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!R$2:R$21) / NormRatings!$L$22 / NormRatings!R$22</f>
+        <v>0.16509168229604235</v>
+      </c>
+      <c r="S12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!S$2:S$21) / NormRatings!$L$22 / NormRatings!S$22</f>
+        <v>-3.0655808299508334E-3</v>
+      </c>
+      <c r="T12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!T$2:T$21) / NormRatings!$L$22 / NormRatings!T$22</f>
+        <v>-0.11267134158707748</v>
+      </c>
+      <c r="U12">
+        <f>SUMPRODUCT(NormRatings!$L$2:$L$21, NormRatings!U$2:U$21) / NormRatings!$L$22 / NormRatings!U$22</f>
+        <v>8.1257459091567674E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!B$2:B$21) / NormRatings!$M$22 / NormRatings!B$22</f>
+        <v>0.18471220265778823</v>
+      </c>
+      <c r="C13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!C$2:C$21) / NormRatings!$M$22 / NormRatings!C$22</f>
+        <v>-3.6622272121207217E-3</v>
+      </c>
+      <c r="D13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!D$2:D$21) / NormRatings!$M$22 / NormRatings!D$22</f>
+        <v>-0.18423079907615575</v>
+      </c>
+      <c r="E13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!E$2:E$21) / NormRatings!$M$22 / NormRatings!E$22</f>
+        <v>-4.9894481494938074E-2</v>
+      </c>
+      <c r="F13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!F$2:F$21) / NormRatings!$M$22 / NormRatings!F$22</f>
+        <v>-0.27600320586083976</v>
+      </c>
+      <c r="G13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!G$2:G$21) / NormRatings!$M$22 / NormRatings!G$22</f>
+        <v>-8.0608567092191774E-2</v>
+      </c>
+      <c r="H13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!H$2:H$21) / NormRatings!$M$22 / NormRatings!H$22</f>
+        <v>-0.22402664855014134</v>
+      </c>
+      <c r="I13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!I$2:I$21) / NormRatings!$M$22 / NormRatings!I$22</f>
+        <v>4.5156230400746296E-2</v>
+      </c>
+      <c r="J13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!J$2:J$21) / NormRatings!$M$22 / NormRatings!J$22</f>
+        <v>-1.3461527896611123E-2</v>
+      </c>
+      <c r="K13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!K$2:K$21) / NormRatings!$M$22 / NormRatings!K$22</f>
+        <v>-9.4090523296631742E-2</v>
+      </c>
+      <c r="L13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!L$2:L$21) / NormRatings!$M$22 / NormRatings!L$22</f>
+        <v>-0.29565422923782619</v>
+      </c>
+      <c r="M13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!M$2:M$21) / NormRatings!$M$22 / NormRatings!M$22</f>
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!N$2:N$21) / NormRatings!$M$22 / NormRatings!N$22</f>
+        <v>-3.2910303143261509E-2</v>
+      </c>
+      <c r="O13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!O$2:O$21) / NormRatings!$M$22 / NormRatings!O$22</f>
+        <v>-0.14843670745743581</v>
+      </c>
+      <c r="P13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!P$2:P$21) / NormRatings!$M$22 / NormRatings!P$22</f>
+        <v>0.38674354377914272</v>
+      </c>
+      <c r="Q13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!Q$2:Q$21) / NormRatings!$M$22 / NormRatings!Q$22</f>
+        <v>-4.7254733493138537E-2</v>
+      </c>
+      <c r="R13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!R$2:R$21) / NormRatings!$M$22 / NormRatings!R$22</f>
+        <v>5.9501438253245054E-2</v>
+      </c>
+      <c r="S13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!S$2:S$21) / NormRatings!$M$22 / NormRatings!S$22</f>
+        <v>-0.22931918062183715</v>
+      </c>
+      <c r="T13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!T$2:T$21) / NormRatings!$M$22 / NormRatings!T$22</f>
+        <v>-0.18807293771490294</v>
+      </c>
+      <c r="U13">
+        <f>SUMPRODUCT(NormRatings!$M$2:$M$21, NormRatings!U$2:U$21) / NormRatings!$M$22 / NormRatings!U$22</f>
+        <v>0.20034130425780752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!B$2:B$21) / NormRatings!$N$22 / NormRatings!B$22</f>
+        <v>-0.31990411258573898</v>
+      </c>
+      <c r="C14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!C$2:C$21) / NormRatings!$N$22 / NormRatings!C$22</f>
+        <v>0.49391225217014634</v>
+      </c>
+      <c r="D14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!D$2:D$21) / NormRatings!$N$22 / NormRatings!D$22</f>
+        <v>-0.19900110135419802</v>
+      </c>
+      <c r="E14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!E$2:E$21) / NormRatings!$N$22 / NormRatings!E$22</f>
+        <v>0.13502180347281489</v>
+      </c>
+      <c r="F14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!F$2:F$21) / NormRatings!$N$22 / NormRatings!F$22</f>
+        <v>0.19636854834003448</v>
+      </c>
+      <c r="G14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!G$2:G$21) / NormRatings!$N$22 / NormRatings!G$22</f>
+        <v>-1.7288710808306108E-2</v>
+      </c>
+      <c r="H14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!H$2:H$21) / NormRatings!$N$22 / NormRatings!H$22</f>
+        <v>-0.61244883080582968</v>
+      </c>
+      <c r="I14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!I$2:I$21) / NormRatings!$N$22 / NormRatings!I$22</f>
+        <v>-0.29114935032904599</v>
+      </c>
+      <c r="J14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!J$2:J$21) / NormRatings!$N$22 / NormRatings!J$22</f>
+        <v>-0.14510149809175904</v>
+      </c>
+      <c r="K14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!K$2:K$21) / NormRatings!$N$22 / NormRatings!K$22</f>
+        <v>3.9140065910084801E-2</v>
+      </c>
+      <c r="L14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!L$2:L$21) / NormRatings!$N$22 / NormRatings!L$22</f>
+        <v>-7.0377526347472519E-2</v>
+      </c>
+      <c r="M14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!M$2:M$21) / NormRatings!$N$22 / NormRatings!M$22</f>
+        <v>-3.2910303143261509E-2</v>
+      </c>
+      <c r="N14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!N$2:N$21) / NormRatings!$N$22 / NormRatings!N$22</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="O14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!O$2:O$21) / NormRatings!$N$22 / NormRatings!O$22</f>
+        <v>0.27408839453101524</v>
+      </c>
+      <c r="P14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!P$2:P$21) / NormRatings!$N$22 / NormRatings!P$22</f>
+        <v>-0.23155340338008884</v>
+      </c>
+      <c r="Q14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!Q$2:Q$21) / NormRatings!$N$22 / NormRatings!Q$22</f>
+        <v>0.12372283370311289</v>
+      </c>
+      <c r="R14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!R$2:R$21) / NormRatings!$N$22 / NormRatings!R$22</f>
+        <v>-0.11617095088617239</v>
+      </c>
+      <c r="S14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!S$2:S$21) / NormRatings!$N$22 / NormRatings!S$22</f>
+        <v>0.39481865444705577</v>
+      </c>
+      <c r="T14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!T$2:T$21) / NormRatings!$N$22 / NormRatings!T$22</f>
+        <v>-0.23752100085348346</v>
+      </c>
+      <c r="U14">
+        <f>SUMPRODUCT(NormRatings!$N$2:$N$21, NormRatings!U$2:U$21) / NormRatings!$N$22 / NormRatings!U$22</f>
+        <v>-0.29427567982670161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!B$2:B$21) / NormRatings!$O$22 / NormRatings!B$22</f>
+        <v>2.000738550895937E-2</v>
+      </c>
+      <c r="C15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!C$2:C$21) / NormRatings!$O$22 / NormRatings!C$22</f>
+        <v>-0.15988213159788864</v>
+      </c>
+      <c r="D15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!D$2:D$21) / NormRatings!$O$22 / NormRatings!D$22</f>
+        <v>-0.15886032348178078</v>
+      </c>
+      <c r="E15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!E$2:E$21) / NormRatings!$O$22 / NormRatings!E$22</f>
+        <v>0.34122912118567678</v>
+      </c>
+      <c r="F15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!F$2:F$21) / NormRatings!$O$22 / NormRatings!F$22</f>
+        <v>2.5442197927654144E-2</v>
+      </c>
+      <c r="G15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!G$2:G$21) / NormRatings!$O$22 / NormRatings!G$22</f>
+        <v>-0.24127474155355685</v>
+      </c>
+      <c r="H15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!H$2:H$21) / NormRatings!$O$22 / NormRatings!H$22</f>
+        <v>-2.9116748707301895E-2</v>
+      </c>
+      <c r="I15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!I$2:I$21) / NormRatings!$O$22 / NormRatings!I$22</f>
+        <v>0.20169374985070959</v>
+      </c>
+      <c r="J15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!J$2:J$21) / NormRatings!$O$22 / NormRatings!J$22</f>
+        <v>-5.1592564238564655E-2</v>
+      </c>
+      <c r="K15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!K$2:K$21) / NormRatings!$O$22 / NormRatings!K$22</f>
+        <v>-0.43639678659297193</v>
+      </c>
+      <c r="L15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!L$2:L$21) / NormRatings!$O$22 / NormRatings!L$22</f>
+        <v>-0.10948502043464493</v>
+      </c>
+      <c r="M15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!M$2:M$21) / NormRatings!$O$22 / NormRatings!M$22</f>
+        <v>-0.14843670745743581</v>
+      </c>
+      <c r="N15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!N$2:N$21) / NormRatings!$O$22 / NormRatings!N$22</f>
+        <v>0.27408839453101524</v>
+      </c>
+      <c r="O15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!O$2:O$21) / NormRatings!$O$22 / NormRatings!O$22</f>
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!P$2:P$21) / NormRatings!$O$22 / NormRatings!P$22</f>
+        <v>-9.7865147126984367E-2</v>
+      </c>
+      <c r="Q15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!Q$2:Q$21) / NormRatings!$O$22 / NormRatings!Q$22</f>
+        <v>-0.24161736441178436</v>
+      </c>
+      <c r="R15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!R$2:R$21) / NormRatings!$O$22 / NormRatings!R$22</f>
+        <v>0.22564260605753822</v>
+      </c>
+      <c r="S15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!S$2:S$21) / NormRatings!$O$22 / NormRatings!S$22</f>
+        <v>8.4705469491518456E-2</v>
+      </c>
+      <c r="T15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!T$2:T$21) / NormRatings!$O$22 / NormRatings!T$22</f>
+        <v>-0.29982283690020606</v>
+      </c>
+      <c r="U15">
+        <f>SUMPRODUCT(NormRatings!$O$2:$O$21, NormRatings!U$2:U$21) / NormRatings!$O$22 / NormRatings!U$22</f>
+        <v>0.1837873696638582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!B$2:B$21) / NormRatings!$P$22 / NormRatings!B$22</f>
+        <v>-0.1055836923612558</v>
+      </c>
+      <c r="C16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!C$2:C$21) / NormRatings!$P$22 / NormRatings!C$22</f>
+        <v>-0.27148913396548996</v>
+      </c>
+      <c r="D16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!D$2:D$21) / NormRatings!$P$22 / NormRatings!D$22</f>
+        <v>-0.25831232083260147</v>
+      </c>
+      <c r="E16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!E$2:E$21) / NormRatings!$P$22 / NormRatings!E$22</f>
+        <v>-0.10128426140629751</v>
+      </c>
+      <c r="F16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!F$2:F$21) / NormRatings!$P$22 / NormRatings!F$22</f>
+        <v>1.1303188058154643E-2</v>
+      </c>
+      <c r="G16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!G$2:G$21) / NormRatings!$P$22 / NormRatings!G$22</f>
+        <v>-0.12845327480426177</v>
+      </c>
+      <c r="H16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!H$2:H$21) / NormRatings!$P$22 / NormRatings!H$22</f>
+        <v>-6.3479295498554827E-2</v>
+      </c>
+      <c r="I16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!I$2:I$21) / NormRatings!$P$22 / NormRatings!I$22</f>
+        <v>0.13606351293652716</v>
+      </c>
+      <c r="J16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!J$2:J$21) / NormRatings!$P$22 / NormRatings!J$22</f>
+        <v>1.8982634310231183E-2</v>
+      </c>
+      <c r="K16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!K$2:K$21) / NormRatings!$P$22 / NormRatings!K$22</f>
+        <v>-0.37381482374619707</v>
+      </c>
+      <c r="L16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!L$2:L$21) / NormRatings!$P$22 / NormRatings!L$22</f>
+        <v>-0.51785889843625921</v>
+      </c>
+      <c r="M16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!M$2:M$21) / NormRatings!$P$22 / NormRatings!M$22</f>
+        <v>0.38674354377914272</v>
+      </c>
+      <c r="N16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!N$2:N$21) / NormRatings!$P$22 / NormRatings!N$22</f>
+        <v>-0.23155340338008884</v>
+      </c>
+      <c r="O16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!O$2:O$21) / NormRatings!$P$22 / NormRatings!O$22</f>
+        <v>-9.7865147126984367E-2</v>
+      </c>
+      <c r="P16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!P$2:P$21) / NormRatings!$P$22 / NormRatings!P$22</f>
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!Q$2:Q$21) / NormRatings!$P$22 / NormRatings!Q$22</f>
+        <v>0.1783431368971535</v>
+      </c>
+      <c r="R16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!R$2:R$21) / NormRatings!$P$22 / NormRatings!R$22</f>
+        <v>-6.2940813452483438E-2</v>
+      </c>
+      <c r="S16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!S$2:S$21) / NormRatings!$P$22 / NormRatings!S$22</f>
+        <v>0.14142726648355755</v>
+      </c>
+      <c r="T16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!T$2:T$21) / NormRatings!$P$22 / NormRatings!T$22</f>
+        <v>-1.0598786952355639E-2</v>
+      </c>
+      <c r="U16">
+        <f>SUMPRODUCT(NormRatings!$P$2:$P$21, NormRatings!U$2:U$21) / NormRatings!$P$22 / NormRatings!U$22</f>
+        <v>0.27377998468037434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!B$2:B$21) / NormRatings!$Q$22 / NormRatings!B$22</f>
+        <v>-0.42033136932878534</v>
+      </c>
+      <c r="C17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!C$2:C$21) / NormRatings!$Q$22 / NormRatings!C$22</f>
+        <v>0.4358847493676889</v>
+      </c>
+      <c r="D17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!D$2:D$21) / NormRatings!$Q$22 / NormRatings!D$22</f>
+        <v>-0.34446330285480997</v>
+      </c>
+      <c r="E17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!E$2:E$21) / NormRatings!$Q$22 / NormRatings!E$22</f>
+        <v>-6.732935070085834E-2</v>
+      </c>
+      <c r="F17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!F$2:F$21) / NormRatings!$Q$22 / NormRatings!F$22</f>
+        <v>0.1803656901652074</v>
+      </c>
+      <c r="G17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!G$2:G$21) / NormRatings!$Q$22 / NormRatings!G$22</f>
+        <v>-0.21773793467394631</v>
+      </c>
+      <c r="H17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!H$2:H$21) / NormRatings!$Q$22 / NormRatings!H$22</f>
+        <v>-0.19215041457752635</v>
+      </c>
+      <c r="I17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!I$2:I$21) / NormRatings!$Q$22 / NormRatings!I$22</f>
+        <v>-0.18719824061676182</v>
+      </c>
+      <c r="J17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!J$2:J$21) / NormRatings!$Q$22 / NormRatings!J$22</f>
+        <v>-0.3486830932414996</v>
+      </c>
+      <c r="K17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!K$2:K$21) / NormRatings!$Q$22 / NormRatings!K$22</f>
+        <v>0.21487516831849041</v>
+      </c>
+      <c r="L17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!L$2:L$21) / NormRatings!$Q$22 / NormRatings!L$22</f>
+        <v>-0.10780486878852018</v>
+      </c>
+      <c r="M17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!M$2:M$21) / NormRatings!$Q$22 / NormRatings!M$22</f>
+        <v>-4.7254733493138537E-2</v>
+      </c>
+      <c r="N17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!N$2:N$21) / NormRatings!$Q$22 / NormRatings!N$22</f>
+        <v>0.12372283370311289</v>
+      </c>
+      <c r="O17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!O$2:O$21) / NormRatings!$Q$22 / NormRatings!O$22</f>
+        <v>-0.24161736441178439</v>
+      </c>
+      <c r="P17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!P$2:P$21) / NormRatings!$Q$22 / NormRatings!P$22</f>
+        <v>0.17834313689715348</v>
+      </c>
+      <c r="Q17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!Q$2:Q$21) / NormRatings!$Q$22 / NormRatings!Q$22</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="R17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!R$2:R$21) / NormRatings!$Q$22 / NormRatings!R$22</f>
+        <v>-0.27675769286489571</v>
+      </c>
+      <c r="S17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!S$2:S$21) / NormRatings!$Q$22 / NormRatings!S$22</f>
+        <v>0.19466816244246957</v>
+      </c>
+      <c r="T17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!T$2:T$21) / NormRatings!$Q$22 / NormRatings!T$22</f>
+        <v>3.702434509564094E-2</v>
+      </c>
+      <c r="U17">
+        <f>SUMPRODUCT(NormRatings!$Q$2:$Q$21, NormRatings!U$2:U$21) / NormRatings!$Q$22 / NormRatings!U$22</f>
+        <v>-0.21629847579240299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!B$2:B$21) / NormRatings!$R$22 / NormRatings!B$22</f>
+        <v>-0.14678361078028837</v>
+      </c>
+      <c r="C18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!C$2:C$21) / NormRatings!$R$22 / NormRatings!C$22</f>
+        <v>-0.25027372858887031</v>
+      </c>
+      <c r="D18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!D$2:D$21) / NormRatings!$R$22 / NormRatings!D$22</f>
+        <v>0.27157977147770279</v>
+      </c>
+      <c r="E18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!E$2:E$21) / NormRatings!$R$22 / NormRatings!E$22</f>
+        <v>-0.21326361555047882</v>
+      </c>
+      <c r="F18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!F$2:F$21) / NormRatings!$R$22 / NormRatings!F$22</f>
+        <v>0.2277775932481598</v>
+      </c>
+      <c r="G18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!G$2:G$21) / NormRatings!$R$22 / NormRatings!G$22</f>
+        <v>-0.27689129094030851</v>
+      </c>
+      <c r="H18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!H$2:H$21) / NormRatings!$R$22 / NormRatings!H$22</f>
+        <v>0.23091237747387072</v>
+      </c>
+      <c r="I18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!I$2:I$21) / NormRatings!$R$22 / NormRatings!I$22</f>
+        <v>0.15849371661451467</v>
+      </c>
+      <c r="J18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!J$2:J$21) / NormRatings!$R$22 / NormRatings!J$22</f>
+        <v>8.8526348280390341E-2</v>
+      </c>
+      <c r="K18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!K$2:K$21) / NormRatings!$R$22 / NormRatings!K$22</f>
+        <v>-8.3199272055368589E-2</v>
+      </c>
+      <c r="L18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!L$2:L$21) / NormRatings!$R$22 / NormRatings!L$22</f>
+        <v>0.16509168229604235</v>
+      </c>
+      <c r="M18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!M$2:M$21) / NormRatings!$R$22 / NormRatings!M$22</f>
+        <v>5.9501438253245061E-2</v>
+      </c>
+      <c r="N18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!N$2:N$21) / NormRatings!$R$22 / NormRatings!N$22</f>
+        <v>-0.11617095088617239</v>
+      </c>
+      <c r="O18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!O$2:O$21) / NormRatings!$R$22 / NormRatings!O$22</f>
+        <v>0.22564260605753825</v>
+      </c>
+      <c r="P18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!P$2:P$21) / NormRatings!$R$22 / NormRatings!P$22</f>
+        <v>-6.2940813452483438E-2</v>
+      </c>
+      <c r="Q18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!Q$2:Q$21) / NormRatings!$R$22 / NormRatings!Q$22</f>
+        <v>-0.27675769286489571</v>
+      </c>
+      <c r="R18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!R$2:R$21) / NormRatings!$R$22 / NormRatings!R$22</f>
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!S$2:S$21) / NormRatings!$R$22 / NormRatings!S$22</f>
+        <v>-0.39175898846746932</v>
+      </c>
+      <c r="T18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!T$2:T$21) / NormRatings!$R$22 / NormRatings!T$22</f>
+        <v>-0.25364967752116241</v>
+      </c>
+      <c r="U18">
+        <f>SUMPRODUCT(NormRatings!$R$2:$R$21, NormRatings!U$2:U$21) / NormRatings!$R$22 / NormRatings!U$22</f>
+        <v>-0.21501514874904057</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!B$2:B$21) / NormRatings!$S$22 / NormRatings!B$22</f>
+        <v>-0.24128093854653215</v>
+      </c>
+      <c r="C19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!C$2:C$21) / NormRatings!$S$22 / NormRatings!C$22</f>
+        <v>1.6440895757123954E-2</v>
+      </c>
+      <c r="D19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!D$2:D$21) / NormRatings!$S$22 / NormRatings!D$22</f>
+        <v>-0.12000690061044302</v>
+      </c>
+      <c r="E19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!E$2:E$21) / NormRatings!$S$22 / NormRatings!E$22</f>
+        <v>-0.26148228822764069</v>
+      </c>
+      <c r="F19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!F$2:F$21) / NormRatings!$S$22 / NormRatings!F$22</f>
+        <v>0.40132014193944721</v>
+      </c>
+      <c r="G19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!G$2:G$21) / NormRatings!$S$22 / NormRatings!G$22</f>
+        <v>0.1314578096042659</v>
+      </c>
+      <c r="H19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!H$2:H$21) / NormRatings!$S$22 / NormRatings!H$22</f>
+        <v>-0.40826013627367458</v>
+      </c>
+      <c r="I19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!I$2:I$21) / NormRatings!$S$22 / NormRatings!I$22</f>
+        <v>-7.1244359962643722E-2</v>
+      </c>
+      <c r="J19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!J$2:J$21) / NormRatings!$S$22 / NormRatings!J$22</f>
+        <v>-0.53011055804302232</v>
+      </c>
+      <c r="K19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!K$2:K$21) / NormRatings!$S$22 / NormRatings!K$22</f>
+        <v>-0.45821341144447997</v>
+      </c>
+      <c r="L19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!L$2:L$21) / NormRatings!$S$22 / NormRatings!L$22</f>
+        <v>-3.0655808299508334E-3</v>
+      </c>
+      <c r="M19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!M$2:M$21) / NormRatings!$S$22 / NormRatings!M$22</f>
+        <v>-0.22931918062183715</v>
+      </c>
+      <c r="N19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!N$2:N$21) / NormRatings!$S$22 / NormRatings!N$22</f>
+        <v>0.39481865444705577</v>
+      </c>
+      <c r="O19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!O$2:O$21) / NormRatings!$S$22 / NormRatings!O$22</f>
+        <v>8.4705469491518456E-2</v>
+      </c>
+      <c r="P19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!P$2:P$21) / NormRatings!$S$22 / NormRatings!P$22</f>
+        <v>0.14142726648355755</v>
+      </c>
+      <c r="Q19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!Q$2:Q$21) / NormRatings!$S$22 / NormRatings!Q$22</f>
+        <v>0.19466816244246954</v>
+      </c>
+      <c r="R19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!R$2:R$21) / NormRatings!$S$22 / NormRatings!R$22</f>
+        <v>-0.39175898846746932</v>
+      </c>
+      <c r="S19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!S$2:S$21) / NormRatings!$S$22 / NormRatings!S$22</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="T19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!T$2:T$21) / NormRatings!$S$22 / NormRatings!T$22</f>
+        <v>0.27406505959575406</v>
+      </c>
+      <c r="U19">
+        <f>SUMPRODUCT(NormRatings!$S$2:$S$21, NormRatings!U$2:U$21) / NormRatings!$S$22 / NormRatings!U$22</f>
+        <v>-3.9267305125561133E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!B$2:B$21) / NormRatings!$T$22 / NormRatings!B$22</f>
+        <v>-0.24885679814496334</v>
+      </c>
+      <c r="C20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!C$2:C$21) / NormRatings!$T$22 / NormRatings!C$22</f>
+        <v>3.8345942402239333E-2</v>
+      </c>
+      <c r="D20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!D$2:D$21) / NormRatings!$T$22 / NormRatings!D$22</f>
+        <v>-7.6493639642324626E-2</v>
+      </c>
+      <c r="E20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!E$2:E$21) / NormRatings!$T$22 / NormRatings!E$22</f>
+        <v>-0.34376595143984073</v>
+      </c>
+      <c r="F20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!F$2:F$21) / NormRatings!$T$22 / NormRatings!F$22</f>
+        <v>-1.0013615857306585E-2</v>
+      </c>
+      <c r="G20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!G$2:G$21) / NormRatings!$T$22 / NormRatings!G$22</f>
+        <v>0.10060165349150764</v>
+      </c>
+      <c r="H20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!H$2:H$21) / NormRatings!$T$22 / NormRatings!H$22</f>
+        <v>0.1848447921524094</v>
+      </c>
+      <c r="I20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!I$2:I$21) / NormRatings!$T$22 / NormRatings!I$22</f>
+        <v>0.331349590586206</v>
+      </c>
+      <c r="J20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!J$2:J$21) / NormRatings!$T$22 / NormRatings!J$22</f>
+        <v>-0.2919826131803987</v>
+      </c>
+      <c r="K20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!K$2:K$21) / NormRatings!$T$22 / NormRatings!K$22</f>
+        <v>5.5206773156534633E-2</v>
+      </c>
+      <c r="L20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!L$2:L$21) / NormRatings!$T$22 / NormRatings!L$22</f>
+        <v>-0.11267134158707748</v>
+      </c>
+      <c r="M20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!M$2:M$21) / NormRatings!$T$22 / NormRatings!M$22</f>
+        <v>-0.18807293771490297</v>
+      </c>
+      <c r="N20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!N$2:N$21) / NormRatings!$T$22 / NormRatings!N$22</f>
+        <v>-0.23752100085348346</v>
+      </c>
+      <c r="O20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!O$2:O$21) / NormRatings!$T$22 / NormRatings!O$22</f>
+        <v>-0.29982283690020606</v>
+      </c>
+      <c r="P20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!P$2:P$21) / NormRatings!$T$22 / NormRatings!P$22</f>
+        <v>-1.0598786952355639E-2</v>
+      </c>
+      <c r="Q20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!Q$2:Q$21) / NormRatings!$T$22 / NormRatings!Q$22</f>
+        <v>3.702434509564094E-2</v>
+      </c>
+      <c r="R20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!R$2:R$21) / NormRatings!$T$22 / NormRatings!R$22</f>
+        <v>-0.25364967752116241</v>
+      </c>
+      <c r="S20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!S$2:S$21) / NormRatings!$T$22 / NormRatings!S$22</f>
+        <v>0.27406505959575406</v>
+      </c>
+      <c r="T20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!T$2:T$21) / NormRatings!$T$22 / NormRatings!T$22</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="U20">
+        <f>SUMPRODUCT(NormRatings!$T$2:$T$21, NormRatings!U$2:U$21) / NormRatings!$T$22 / NormRatings!U$22</f>
+        <v>-0.20788538974311041</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!B$2:B$21) / NormRatings!$U$22 / NormRatings!B$22</f>
+        <v>0.55444750193353987</v>
+      </c>
+      <c r="C21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!C$2:C$21) / NormRatings!$U$22 / NormRatings!C$22</f>
+        <v>-0.32287453355402224</v>
+      </c>
+      <c r="D21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!D$2:D$21) / NormRatings!$U$22 / NormRatings!D$22</f>
+        <v>-0.24015520716514135</v>
+      </c>
+      <c r="E21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!E$2:E$21) / NormRatings!$U$22 / NormRatings!E$22</f>
+        <v>0.32353240190383042</v>
+      </c>
+      <c r="F21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!F$2:F$21) / NormRatings!$U$22 / NormRatings!F$22</f>
+        <v>-0.45992867072689786</v>
+      </c>
+      <c r="G21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!G$2:G$21) / NormRatings!$U$22 / NormRatings!G$22</f>
+        <v>-0.18024862598365846</v>
+      </c>
+      <c r="H21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!H$2:H$21) / NormRatings!$U$22 / NormRatings!H$22</f>
+        <v>9.5852757712291584E-2</v>
+      </c>
+      <c r="I21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!I$2:I$21) / NormRatings!$U$22 / NormRatings!I$22</f>
+        <v>6.9644128532871608E-2</v>
+      </c>
+      <c r="J21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!J$2:J$21) / NormRatings!$U$22 / NormRatings!J$22</f>
+        <v>0.26172689797317195</v>
+      </c>
+      <c r="K21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!K$2:K$21) / NormRatings!$U$22 / NormRatings!K$22</f>
+        <v>-0.58553091006906921</v>
+      </c>
+      <c r="L21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!L$2:L$21) / NormRatings!$U$22 / NormRatings!L$22</f>
+        <v>8.1257459091567674E-3</v>
+      </c>
+      <c r="M21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!M$2:M$21) / NormRatings!$U$22 / NormRatings!M$22</f>
+        <v>0.20034130425780755</v>
+      </c>
+      <c r="N21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!N$2:N$21) / NormRatings!$U$22 / NormRatings!N$22</f>
+        <v>-0.29427567982670155</v>
+      </c>
+      <c r="O21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!O$2:O$21) / NormRatings!$U$22 / NormRatings!O$22</f>
+        <v>0.18378736966385822</v>
+      </c>
+      <c r="P21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!P$2:P$21) / NormRatings!$U$22 / NormRatings!P$22</f>
+        <v>0.2737799846803744</v>
+      </c>
+      <c r="Q21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!Q$2:Q$21) / NormRatings!$U$22 / NormRatings!Q$22</f>
+        <v>-0.21629847579240302</v>
+      </c>
+      <c r="R21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!R$2:R$21) / NormRatings!$U$22 / NormRatings!R$22</f>
+        <v>-0.21501514874904057</v>
+      </c>
+      <c r="S21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!S$2:S$21) / NormRatings!$U$22 / NormRatings!S$22</f>
+        <v>-3.9267305125561126E-2</v>
+      </c>
+      <c r="T21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!T$2:T$21) / NormRatings!$U$22 / NormRatings!T$22</f>
+        <v>-0.20788538974311041</v>
+      </c>
+      <c r="U21">
+        <f>SUMPRODUCT(NormRatings!$U$2:$U$21, NormRatings!U$2:U$21) / NormRatings!$U$22 / NormRatings!U$22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:U21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CE2943-F9C7-2D4E-B536-8569BAE68B47}">
+  <dimension ref="A1:U44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
+        <f>MAX(NormMatrix!B2,0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C2" s="4">
+        <f>MAX(NormMatrix!C2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <f>MAX(NormMatrix!D2,0)</f>
+        <v>0.35577972454766571</v>
+      </c>
+      <c r="E2" s="4">
+        <f>MAX(NormMatrix!E2,0)</f>
+        <v>0.21597537370665254</v>
+      </c>
+      <c r="F2" s="4">
+        <f>MAX(NormMatrix!F2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <f>MAX(NormMatrix!G2,0)</f>
+        <v>0.13921371111490649</v>
+      </c>
+      <c r="H2" s="4">
+        <f>MAX(NormMatrix!H2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <f>MAX(NormMatrix!I2,0)</f>
+        <v>0.19279858482944665</v>
+      </c>
+      <c r="J2" s="4">
+        <f>MAX(NormMatrix!J2,0)</f>
+        <v>0.29501316508704811</v>
+      </c>
+      <c r="K2" s="4">
+        <f>MAX(NormMatrix!K2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <f>MAX(NormMatrix!L2,0)</f>
+        <v>0.11675543916439571</v>
+      </c>
+      <c r="M2" s="4">
+        <f>MAX(NormMatrix!M2,0)</f>
+        <v>0.18471220265778823</v>
+      </c>
+      <c r="N2" s="4">
+        <f>MAX(NormMatrix!N2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <f>MAX(NormMatrix!O2,0)</f>
+        <v>2.0007385508959367E-2</v>
+      </c>
+      <c r="P2" s="4">
+        <f>MAX(NormMatrix!P2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>MAX(NormMatrix!Q2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="4">
+        <f>MAX(NormMatrix!R2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <f>MAX(NormMatrix!S2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <f>MAX(NormMatrix!T2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="4">
+        <f>MAX(NormMatrix!U2,0)</f>
+        <v>0.55444750193353987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <f>MAX(NormMatrix!B3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <f>MAX(NormMatrix!C3,0)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="D3" s="4">
+        <f>MAX(NormMatrix!D3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <f>MAX(NormMatrix!E3,0)</f>
+        <v>3.5870569165431928E-3</v>
+      </c>
+      <c r="F3" s="4">
+        <f>MAX(NormMatrix!F3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <f>MAX(NormMatrix!G3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <f>MAX(NormMatrix!H3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <f>MAX(NormMatrix!I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <f>MAX(NormMatrix!J3,0)</f>
+        <v>1.3543190284680795E-2</v>
+      </c>
+      <c r="K3" s="4">
+        <f>MAX(NormMatrix!K3,0)</f>
+        <v>0.31518507647562766</v>
+      </c>
+      <c r="L3" s="4">
+        <f>MAX(NormMatrix!L3,0)</f>
+        <v>0.15540846526009983</v>
+      </c>
+      <c r="M3" s="4">
+        <f>MAX(NormMatrix!M3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <f>MAX(NormMatrix!N3,0)</f>
+        <v>0.49391225217014639</v>
+      </c>
+      <c r="O3" s="4">
+        <f>MAX(NormMatrix!O3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <f>MAX(NormMatrix!P3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>MAX(NormMatrix!Q3,0)</f>
+        <v>0.43588474936768895</v>
+      </c>
+      <c r="R3" s="4">
+        <f>MAX(NormMatrix!R3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <f>MAX(NormMatrix!S3,0)</f>
+        <v>1.6440895757123954E-2</v>
+      </c>
+      <c r="T3" s="4">
+        <f>MAX(NormMatrix!T3,0)</f>
+        <v>3.8345942402239333E-2</v>
+      </c>
+      <c r="U3" s="4">
+        <f>MAX(NormMatrix!U3,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <f>MAX(NormMatrix!B4,0)</f>
+        <v>0.35577972454766577</v>
+      </c>
+      <c r="C4" s="4">
+        <f>MAX(NormMatrix!C4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <f>MAX(NormMatrix!D4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <f>MAX(NormMatrix!E4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f>MAX(NormMatrix!F4,0)</f>
+        <v>2.3469953903822744E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <f>MAX(NormMatrix!G4,0)</f>
+        <v>0.39156391871191337</v>
+      </c>
+      <c r="H4" s="4">
+        <f>MAX(NormMatrix!H4,0)</f>
+        <v>0.10094588826430767</v>
+      </c>
+      <c r="I4" s="4">
+        <f>MAX(NormMatrix!I4,0)</f>
+        <v>7.5201233799563505E-2</v>
+      </c>
+      <c r="J4" s="4">
+        <f>MAX(NormMatrix!J4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <f>MAX(NormMatrix!K4,0)</f>
+        <v>0.1940588267347674</v>
+      </c>
+      <c r="L4" s="4">
+        <f>MAX(NormMatrix!L4,0)</f>
+        <v>0.13382387317628316</v>
+      </c>
+      <c r="M4" s="4">
+        <f>MAX(NormMatrix!M4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <f>MAX(NormMatrix!N4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <f>MAX(NormMatrix!O4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <f>MAX(NormMatrix!P4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>MAX(NormMatrix!Q4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <f>MAX(NormMatrix!R4,0)</f>
+        <v>0.27157977147770279</v>
+      </c>
+      <c r="S4" s="4">
+        <f>MAX(NormMatrix!S4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <f>MAX(NormMatrix!T4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <f>MAX(NormMatrix!U4,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <f>MAX(NormMatrix!B5,0)</f>
+        <v>0.21597537370665254</v>
+      </c>
+      <c r="C5" s="4">
+        <f>MAX(NormMatrix!C5,0)</f>
+        <v>3.5870569165431928E-3</v>
+      </c>
+      <c r="D5" s="4">
+        <f>MAX(NormMatrix!D5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <f>MAX(NormMatrix!E5,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <f>MAX(NormMatrix!F5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <f>MAX(NormMatrix!G5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <f>MAX(NormMatrix!H5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <f>MAX(NormMatrix!I5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <f>MAX(NormMatrix!J5,0)</f>
+        <v>0.34361515261779119</v>
+      </c>
+      <c r="K5" s="4">
+        <f>MAX(NormMatrix!K5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <f>MAX(NormMatrix!L5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <f>MAX(NormMatrix!M5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f>MAX(NormMatrix!N5,0)</f>
+        <v>0.13502180347281489</v>
+      </c>
+      <c r="O5" s="4">
+        <f>MAX(NormMatrix!O5,0)</f>
+        <v>0.34122912118567683</v>
+      </c>
+      <c r="P5" s="4">
+        <f>MAX(NormMatrix!P5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>MAX(NormMatrix!Q5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <f>MAX(NormMatrix!R5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <f>MAX(NormMatrix!S5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="4">
+        <f>MAX(NormMatrix!T5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="4">
+        <f>MAX(NormMatrix!U5,0)</f>
+        <v>0.32353240190383042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <f>MAX(NormMatrix!B6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <f>MAX(NormMatrix!C6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <f>MAX(NormMatrix!D6,0)</f>
+        <v>2.3469953903822744E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <f>MAX(NormMatrix!E6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <f>MAX(NormMatrix!F6,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <f>MAX(NormMatrix!G6,0)</f>
+        <v>8.8281840279244864E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <f>MAX(NormMatrix!H6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <f>MAX(NormMatrix!I6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <f>MAX(NormMatrix!J6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <f>MAX(NormMatrix!K6,0)</f>
+        <v>0.11286299690121732</v>
+      </c>
+      <c r="L6" s="4">
+        <f>MAX(NormMatrix!L6,0)</f>
+        <v>8.9045163112599843E-2</v>
+      </c>
+      <c r="M6" s="4">
+        <f>MAX(NormMatrix!M6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <f>MAX(NormMatrix!N6,0)</f>
+        <v>0.19636854834003448</v>
+      </c>
+      <c r="O6" s="4">
+        <f>MAX(NormMatrix!O6,0)</f>
+        <v>2.5442197927654141E-2</v>
+      </c>
+      <c r="P6" s="4">
+        <f>MAX(NormMatrix!P6,0)</f>
+        <v>1.1303188058154643E-2</v>
+      </c>
+      <c r="Q6" s="4">
+        <f>MAX(NormMatrix!Q6,0)</f>
+        <v>0.1803656901652074</v>
+      </c>
+      <c r="R6" s="4">
+        <f>MAX(NormMatrix!R6,0)</f>
+        <v>0.2277775932481598</v>
+      </c>
+      <c r="S6" s="4">
+        <f>MAX(NormMatrix!S6,0)</f>
+        <v>0.40132014193944721</v>
+      </c>
+      <c r="T6" s="4">
+        <f>MAX(NormMatrix!T6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="4">
+        <f>MAX(NormMatrix!U6,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <f>MAX(NormMatrix!B7,0)</f>
+        <v>0.13921371111490652</v>
+      </c>
+      <c r="C7" s="4">
+        <f>MAX(NormMatrix!C7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <f>MAX(NormMatrix!D7,0)</f>
+        <v>0.39156391871191343</v>
+      </c>
+      <c r="E7" s="4">
+        <f>MAX(NormMatrix!E7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <f>MAX(NormMatrix!F7,0)</f>
+        <v>8.8281840279244864E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <f>MAX(NormMatrix!G7,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <f>MAX(NormMatrix!H7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <f>MAX(NormMatrix!I7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <f>MAX(NormMatrix!J7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <f>MAX(NormMatrix!K7,0)</f>
+        <v>0.27830998560508052</v>
+      </c>
+      <c r="L7" s="4">
+        <f>MAX(NormMatrix!L7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <f>MAX(NormMatrix!M7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <f>MAX(NormMatrix!N7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <f>MAX(NormMatrix!O7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <f>MAX(NormMatrix!P7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>MAX(NormMatrix!Q7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <f>MAX(NormMatrix!R7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f>MAX(NormMatrix!S7,0)</f>
+        <v>0.1314578096042659</v>
+      </c>
+      <c r="T7" s="4">
+        <f>MAX(NormMatrix!T7,0)</f>
+        <v>0.10060165349150764</v>
+      </c>
+      <c r="U7" s="4">
+        <f>MAX(NormMatrix!U7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <f>MAX(NormMatrix!B8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <f>MAX(NormMatrix!C8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <f>MAX(NormMatrix!D8,0)</f>
+        <v>0.10094588826430768</v>
+      </c>
+      <c r="E8" s="4">
+        <f>MAX(NormMatrix!E8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <f>MAX(NormMatrix!F8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <f>MAX(NormMatrix!G8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <f>MAX(NormMatrix!H8,0)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I8" s="4">
+        <f>MAX(NormMatrix!I8,0)</f>
+        <v>0.17472391669004284</v>
+      </c>
+      <c r="J8" s="4">
+        <f>MAX(NormMatrix!J8,0)</f>
+        <v>0.19190832656287304</v>
+      </c>
+      <c r="K8" s="4">
+        <f>MAX(NormMatrix!K8,0)</f>
+        <v>7.0879871588571536E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <f>MAX(NormMatrix!L8,0)</f>
+        <v>0.1308552371719458</v>
+      </c>
+      <c r="M8" s="4">
+        <f>MAX(NormMatrix!M8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <f>MAX(NormMatrix!N8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <f>MAX(NormMatrix!O8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <f>MAX(NormMatrix!P8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>MAX(NormMatrix!Q8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <f>MAX(NormMatrix!R8,0)</f>
+        <v>0.23091237747387072</v>
+      </c>
+      <c r="S8" s="4">
+        <f>MAX(NormMatrix!S8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <f>MAX(NormMatrix!T8,0)</f>
+        <v>0.18484479215240943</v>
+      </c>
+      <c r="U8" s="4">
+        <f>MAX(NormMatrix!U8,0)</f>
+        <v>9.585275771229157E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <f>MAX(NormMatrix!B9,0)</f>
+        <v>0.19279858482944665</v>
+      </c>
+      <c r="C9" s="4">
+        <f>MAX(NormMatrix!C9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <f>MAX(NormMatrix!D9,0)</f>
+        <v>7.5201233799563519E-2</v>
+      </c>
+      <c r="E9" s="4">
+        <f>MAX(NormMatrix!E9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <f>MAX(NormMatrix!F9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <f>MAX(NormMatrix!G9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>MAX(NormMatrix!H9,0)</f>
+        <v>0.17472391669004284</v>
+      </c>
+      <c r="I9" s="4">
+        <f>MAX(NormMatrix!I9,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <f>MAX(NormMatrix!J9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <f>MAX(NormMatrix!K9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <f>MAX(NormMatrix!L9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <f>MAX(NormMatrix!M9,0)</f>
+        <v>4.5156230400746289E-2</v>
+      </c>
+      <c r="N9" s="4">
+        <f>MAX(NormMatrix!N9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <f>MAX(NormMatrix!O9,0)</f>
+        <v>0.20169374985070956</v>
+      </c>
+      <c r="P9" s="4">
+        <f>MAX(NormMatrix!P9,0)</f>
+        <v>0.13606351293652716</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>MAX(NormMatrix!Q9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <f>MAX(NormMatrix!R9,0)</f>
+        <v>0.15849371661451467</v>
+      </c>
+      <c r="S9" s="4">
+        <f>MAX(NormMatrix!S9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <f>MAX(NormMatrix!T9,0)</f>
+        <v>0.331349590586206</v>
+      </c>
+      <c r="U9" s="4">
+        <f>MAX(NormMatrix!U9,0)</f>
+        <v>6.9644128532871608E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <f>MAX(NormMatrix!B10,0)</f>
+        <v>0.29501316508704806</v>
+      </c>
+      <c r="C10" s="4">
+        <f>MAX(NormMatrix!C10,0)</f>
+        <v>1.3543190284680796E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <f>MAX(NormMatrix!D10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <f>MAX(NormMatrix!E10,0)</f>
+        <v>0.34361515261779119</v>
+      </c>
+      <c r="F10" s="4">
+        <f>MAX(NormMatrix!F10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <f>MAX(NormMatrix!G10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>MAX(NormMatrix!H10,0)</f>
+        <v>0.19190832656287307</v>
+      </c>
+      <c r="I10" s="4">
+        <f>MAX(NormMatrix!I10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <f>MAX(NormMatrix!J10,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <f>MAX(NormMatrix!K10,0)</f>
+        <v>0.12081715289101295</v>
+      </c>
+      <c r="L10" s="4">
+        <f>MAX(NormMatrix!L10,0)</f>
+        <v>0.32648908513771746</v>
+      </c>
+      <c r="M10" s="4">
+        <f>MAX(NormMatrix!M10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <f>MAX(NormMatrix!N10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <f>MAX(NormMatrix!O10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <f>MAX(NormMatrix!P10,0)</f>
+        <v>1.8982634310231183E-2</v>
+      </c>
+      <c r="Q10" s="4">
+        <f>MAX(NormMatrix!Q10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <f>MAX(NormMatrix!R10,0)</f>
+        <v>8.8526348280390341E-2</v>
+      </c>
+      <c r="S10" s="4">
+        <f>MAX(NormMatrix!S10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <f>MAX(NormMatrix!T10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <f>MAX(NormMatrix!U10,0)</f>
+        <v>0.26172689797317195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <f>MAX(NormMatrix!B11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <f>MAX(NormMatrix!C11,0)</f>
+        <v>0.31518507647562766</v>
+      </c>
+      <c r="D11" s="4">
+        <f>MAX(NormMatrix!D11,0)</f>
+        <v>0.19405882673476738</v>
+      </c>
+      <c r="E11" s="4">
+        <f>MAX(NormMatrix!E11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <f>MAX(NormMatrix!F11,0)</f>
+        <v>0.11286299690121732</v>
+      </c>
+      <c r="G11" s="4">
+        <f>MAX(NormMatrix!G11,0)</f>
+        <v>0.27830998560508052</v>
+      </c>
+      <c r="H11" s="4">
+        <f>MAX(NormMatrix!H11,0)</f>
+        <v>7.0879871588571536E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <f>MAX(NormMatrix!I11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <f>MAX(NormMatrix!J11,0)</f>
+        <v>0.12081715289101294</v>
+      </c>
+      <c r="K11" s="4">
+        <f>MAX(NormMatrix!K11,0)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="L11" s="4">
+        <f>MAX(NormMatrix!L11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <f>MAX(NormMatrix!M11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <f>MAX(NormMatrix!N11,0)</f>
+        <v>3.9140065910084794E-2</v>
+      </c>
+      <c r="O11" s="4">
+        <f>MAX(NormMatrix!O11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <f>MAX(NormMatrix!P11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <f>MAX(NormMatrix!Q11,0)</f>
+        <v>0.21487516831849043</v>
+      </c>
+      <c r="R11" s="4">
+        <f>MAX(NormMatrix!R11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <f>MAX(NormMatrix!S11,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <f>MAX(NormMatrix!T11,0)</f>
+        <v>5.520677315653464E-2</v>
+      </c>
+      <c r="U11" s="4">
+        <f>MAX(NormMatrix!U11,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <f>MAX(NormMatrix!B12,0)</f>
+        <v>0.11675543916439569</v>
+      </c>
+      <c r="C12" s="4">
+        <f>MAX(NormMatrix!C12,0)</f>
+        <v>0.15540846526009983</v>
+      </c>
+      <c r="D12" s="4">
+        <f>MAX(NormMatrix!D12,0)</f>
+        <v>0.13382387317628316</v>
+      </c>
+      <c r="E12" s="4">
+        <f>MAX(NormMatrix!E12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <f>MAX(NormMatrix!F12,0)</f>
+        <v>8.9045163112599843E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <f>MAX(NormMatrix!G12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <f>MAX(NormMatrix!H12,0)</f>
+        <v>0.1308552371719458</v>
+      </c>
+      <c r="I12" s="4">
+        <f>MAX(NormMatrix!I12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <f>MAX(NormMatrix!J12,0)</f>
+        <v>0.32648908513771746</v>
+      </c>
+      <c r="K12" s="4">
+        <f>MAX(NormMatrix!K12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <f>MAX(NormMatrix!L12,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="4">
+        <f>MAX(NormMatrix!M12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <f>MAX(NormMatrix!N12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <f>MAX(NormMatrix!O12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <f>MAX(NormMatrix!P12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <f>MAX(NormMatrix!Q12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <f>MAX(NormMatrix!R12,0)</f>
+        <v>0.16509168229604235</v>
+      </c>
+      <c r="S12" s="4">
+        <f>MAX(NormMatrix!S12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
+        <f>MAX(NormMatrix!T12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <f>MAX(NormMatrix!U12,0)</f>
+        <v>8.1257459091567674E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <f>MAX(NormMatrix!B13,0)</f>
+        <v>0.18471220265778823</v>
+      </c>
+      <c r="C13" s="4">
+        <f>MAX(NormMatrix!C13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <f>MAX(NormMatrix!D13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <f>MAX(NormMatrix!E13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <f>MAX(NormMatrix!F13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <f>MAX(NormMatrix!G13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <f>MAX(NormMatrix!H13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <f>MAX(NormMatrix!I13,0)</f>
+        <v>4.5156230400746296E-2</v>
+      </c>
+      <c r="J13" s="4">
+        <f>MAX(NormMatrix!J13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <f>MAX(NormMatrix!K13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <f>MAX(NormMatrix!L13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <f>MAX(NormMatrix!M13,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="4">
+        <f>MAX(NormMatrix!N13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <f>MAX(NormMatrix!O13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <f>MAX(NormMatrix!P13,0)</f>
+        <v>0.38674354377914272</v>
+      </c>
+      <c r="Q13" s="4">
+        <f>MAX(NormMatrix!Q13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <f>MAX(NormMatrix!R13,0)</f>
+        <v>5.9501438253245054E-2</v>
+      </c>
+      <c r="S13" s="4">
+        <f>MAX(NormMatrix!S13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="4">
+        <f>MAX(NormMatrix!T13,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="4">
+        <f>MAX(NormMatrix!U13,0)</f>
+        <v>0.20034130425780752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <f>MAX(NormMatrix!B14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <f>MAX(NormMatrix!C14,0)</f>
+        <v>0.49391225217014634</v>
+      </c>
+      <c r="D14" s="4">
+        <f>MAX(NormMatrix!D14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <f>MAX(NormMatrix!E14,0)</f>
+        <v>0.13502180347281489</v>
+      </c>
+      <c r="F14" s="4">
+        <f>MAX(NormMatrix!F14,0)</f>
+        <v>0.19636854834003448</v>
+      </c>
+      <c r="G14" s="4">
+        <f>MAX(NormMatrix!G14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f>MAX(NormMatrix!H14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <f>MAX(NormMatrix!I14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <f>MAX(NormMatrix!J14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <f>MAX(NormMatrix!K14,0)</f>
+        <v>3.9140065910084801E-2</v>
+      </c>
+      <c r="L14" s="4">
+        <f>MAX(NormMatrix!L14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <f>MAX(NormMatrix!M14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <f>MAX(NormMatrix!N14,0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="O14" s="4">
+        <f>MAX(NormMatrix!O14,0)</f>
+        <v>0.27408839453101524</v>
+      </c>
+      <c r="P14" s="4">
+        <f>MAX(NormMatrix!P14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4">
+        <f>MAX(NormMatrix!Q14,0)</f>
+        <v>0.12372283370311289</v>
+      </c>
+      <c r="R14" s="4">
+        <f>MAX(NormMatrix!R14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="4">
+        <f>MAX(NormMatrix!S14,0)</f>
+        <v>0.39481865444705577</v>
+      </c>
+      <c r="T14" s="4">
+        <f>MAX(NormMatrix!T14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <f>MAX(NormMatrix!U14,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <f>MAX(NormMatrix!B15,0)</f>
+        <v>2.000738550895937E-2</v>
+      </c>
+      <c r="C15" s="4">
+        <f>MAX(NormMatrix!C15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <f>MAX(NormMatrix!D15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <f>MAX(NormMatrix!E15,0)</f>
+        <v>0.34122912118567678</v>
+      </c>
+      <c r="F15" s="4">
+        <f>MAX(NormMatrix!F15,0)</f>
+        <v>2.5442197927654144E-2</v>
+      </c>
+      <c r="G15" s="4">
+        <f>MAX(NormMatrix!G15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <f>MAX(NormMatrix!H15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <f>MAX(NormMatrix!I15,0)</f>
+        <v>0.20169374985070959</v>
+      </c>
+      <c r="J15" s="4">
+        <f>MAX(NormMatrix!J15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <f>MAX(NormMatrix!K15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <f>MAX(NormMatrix!L15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <f>MAX(NormMatrix!M15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <f>MAX(NormMatrix!N15,0)</f>
+        <v>0.27408839453101524</v>
+      </c>
+      <c r="O15" s="4">
+        <f>MAX(NormMatrix!O15,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P15" s="4">
+        <f>MAX(NormMatrix!P15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <f>MAX(NormMatrix!Q15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <f>MAX(NormMatrix!R15,0)</f>
+        <v>0.22564260605753822</v>
+      </c>
+      <c r="S15" s="4">
+        <f>MAX(NormMatrix!S15,0)</f>
+        <v>8.4705469491518456E-2</v>
+      </c>
+      <c r="T15" s="4">
+        <f>MAX(NormMatrix!T15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <f>MAX(NormMatrix!U15,0)</f>
+        <v>0.1837873696638582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <f>MAX(NormMatrix!B16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <f>MAX(NormMatrix!C16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <f>MAX(NormMatrix!D16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <f>MAX(NormMatrix!E16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <f>MAX(NormMatrix!F16,0)</f>
+        <v>1.1303188058154643E-2</v>
+      </c>
+      <c r="G16" s="4">
+        <f>MAX(NormMatrix!G16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <f>MAX(NormMatrix!H16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <f>MAX(NormMatrix!I16,0)</f>
+        <v>0.13606351293652716</v>
+      </c>
+      <c r="J16" s="4">
+        <f>MAX(NormMatrix!J16,0)</f>
+        <v>1.8982634310231183E-2</v>
+      </c>
+      <c r="K16" s="4">
+        <f>MAX(NormMatrix!K16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <f>MAX(NormMatrix!L16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <f>MAX(NormMatrix!M16,0)</f>
+        <v>0.38674354377914272</v>
+      </c>
+      <c r="N16" s="4">
+        <f>MAX(NormMatrix!N16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <f>MAX(NormMatrix!O16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <f>MAX(NormMatrix!P16,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="4">
+        <f>MAX(NormMatrix!Q16,0)</f>
+        <v>0.1783431368971535</v>
+      </c>
+      <c r="R16" s="4">
+        <f>MAX(NormMatrix!R16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <f>MAX(NormMatrix!S16,0)</f>
+        <v>0.14142726648355755</v>
+      </c>
+      <c r="T16" s="4">
+        <f>MAX(NormMatrix!T16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <f>MAX(NormMatrix!U16,0)</f>
+        <v>0.27377998468037434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <f>MAX(NormMatrix!B17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <f>MAX(NormMatrix!C17,0)</f>
+        <v>0.4358847493676889</v>
+      </c>
+      <c r="D17" s="4">
+        <f>MAX(NormMatrix!D17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <f>MAX(NormMatrix!E17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <f>MAX(NormMatrix!F17,0)</f>
+        <v>0.1803656901652074</v>
+      </c>
+      <c r="G17" s="4">
+        <f>MAX(NormMatrix!G17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <f>MAX(NormMatrix!H17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <f>MAX(NormMatrix!I17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <f>MAX(NormMatrix!J17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <f>MAX(NormMatrix!K17,0)</f>
+        <v>0.21487516831849041</v>
+      </c>
+      <c r="L17" s="4">
+        <f>MAX(NormMatrix!L17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <f>MAX(NormMatrix!M17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <f>MAX(NormMatrix!N17,0)</f>
+        <v>0.12372283370311289</v>
+      </c>
+      <c r="O17" s="4">
+        <f>MAX(NormMatrix!O17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <f>MAX(NormMatrix!P17,0)</f>
+        <v>0.17834313689715348</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>MAX(NormMatrix!Q17,0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="R17" s="4">
+        <f>MAX(NormMatrix!R17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <f>MAX(NormMatrix!S17,0)</f>
+        <v>0.19466816244246957</v>
+      </c>
+      <c r="T17" s="4">
+        <f>MAX(NormMatrix!T17,0)</f>
+        <v>3.702434509564094E-2</v>
+      </c>
+      <c r="U17" s="4">
+        <f>MAX(NormMatrix!U17,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <f>MAX(NormMatrix!B18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <f>MAX(NormMatrix!C18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <f>MAX(NormMatrix!D18,0)</f>
+        <v>0.27157977147770279</v>
+      </c>
+      <c r="E18" s="4">
+        <f>MAX(NormMatrix!E18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <f>MAX(NormMatrix!F18,0)</f>
+        <v>0.2277775932481598</v>
+      </c>
+      <c r="G18" s="4">
+        <f>MAX(NormMatrix!G18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <f>MAX(NormMatrix!H18,0)</f>
+        <v>0.23091237747387072</v>
+      </c>
+      <c r="I18" s="4">
+        <f>MAX(NormMatrix!I18,0)</f>
+        <v>0.15849371661451467</v>
+      </c>
+      <c r="J18" s="4">
+        <f>MAX(NormMatrix!J18,0)</f>
+        <v>8.8526348280390341E-2</v>
+      </c>
+      <c r="K18" s="4">
+        <f>MAX(NormMatrix!K18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <f>MAX(NormMatrix!L18,0)</f>
+        <v>0.16509168229604235</v>
+      </c>
+      <c r="M18" s="4">
+        <f>MAX(NormMatrix!M18,0)</f>
+        <v>5.9501438253245061E-2</v>
+      </c>
+      <c r="N18" s="4">
+        <f>MAX(NormMatrix!N18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <f>MAX(NormMatrix!O18,0)</f>
+        <v>0.22564260605753825</v>
+      </c>
+      <c r="P18" s="4">
+        <f>MAX(NormMatrix!P18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4">
+        <f>MAX(NormMatrix!Q18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <f>MAX(NormMatrix!R18,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S18" s="4">
+        <f>MAX(NormMatrix!S18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <f>MAX(NormMatrix!T18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <f>MAX(NormMatrix!U18,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <f>MAX(NormMatrix!B19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <f>MAX(NormMatrix!C19,0)</f>
+        <v>1.6440895757123954E-2</v>
+      </c>
+      <c r="D19" s="4">
+        <f>MAX(NormMatrix!D19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <f>MAX(NormMatrix!E19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <f>MAX(NormMatrix!F19,0)</f>
+        <v>0.40132014193944721</v>
+      </c>
+      <c r="G19" s="4">
+        <f>MAX(NormMatrix!G19,0)</f>
+        <v>0.1314578096042659</v>
+      </c>
+      <c r="H19" s="4">
+        <f>MAX(NormMatrix!H19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <f>MAX(NormMatrix!I19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <f>MAX(NormMatrix!J19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <f>MAX(NormMatrix!K19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <f>MAX(NormMatrix!L19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <f>MAX(NormMatrix!M19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <f>MAX(NormMatrix!N19,0)</f>
+        <v>0.39481865444705577</v>
+      </c>
+      <c r="O19" s="4">
+        <f>MAX(NormMatrix!O19,0)</f>
+        <v>8.4705469491518456E-2</v>
+      </c>
+      <c r="P19" s="4">
+        <f>MAX(NormMatrix!P19,0)</f>
+        <v>0.14142726648355755</v>
+      </c>
+      <c r="Q19" s="4">
+        <f>MAX(NormMatrix!Q19,0)</f>
+        <v>0.19466816244246954</v>
+      </c>
+      <c r="R19" s="4">
+        <f>MAX(NormMatrix!R19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <f>MAX(NormMatrix!S19,0)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="T19" s="4">
+        <f>MAX(NormMatrix!T19,0)</f>
+        <v>0.27406505959575406</v>
+      </c>
+      <c r="U19" s="4">
+        <f>MAX(NormMatrix!U19,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <f>MAX(NormMatrix!B20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <f>MAX(NormMatrix!C20,0)</f>
+        <v>3.8345942402239333E-2</v>
+      </c>
+      <c r="D20" s="4">
+        <f>MAX(NormMatrix!D20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <f>MAX(NormMatrix!E20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <f>MAX(NormMatrix!F20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <f>MAX(NormMatrix!G20,0)</f>
+        <v>0.10060165349150764</v>
+      </c>
+      <c r="H20" s="4">
+        <f>MAX(NormMatrix!H20,0)</f>
+        <v>0.1848447921524094</v>
+      </c>
+      <c r="I20" s="4">
+        <f>MAX(NormMatrix!I20,0)</f>
+        <v>0.331349590586206</v>
+      </c>
+      <c r="J20" s="4">
+        <f>MAX(NormMatrix!J20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <f>MAX(NormMatrix!K20,0)</f>
+        <v>5.5206773156534633E-2</v>
+      </c>
+      <c r="L20" s="4">
+        <f>MAX(NormMatrix!L20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <f>MAX(NormMatrix!M20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <f>MAX(NormMatrix!N20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <f>MAX(NormMatrix!O20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="4">
+        <f>MAX(NormMatrix!P20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="4">
+        <f>MAX(NormMatrix!Q20,0)</f>
+        <v>3.702434509564094E-2</v>
+      </c>
+      <c r="R20" s="4">
+        <f>MAX(NormMatrix!R20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <f>MAX(NormMatrix!S20,0)</f>
+        <v>0.27406505959575406</v>
+      </c>
+      <c r="T20" s="4">
+        <f>MAX(NormMatrix!T20,0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="U20" s="4">
+        <f>MAX(NormMatrix!U20,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
+        <f>MAX(NormMatrix!B21,0)</f>
+        <v>0.55444750193353987</v>
+      </c>
+      <c r="C21" s="6">
+        <f>MAX(NormMatrix!C21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <f>MAX(NormMatrix!D21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <f>MAX(NormMatrix!E21,0)</f>
+        <v>0.32353240190383042</v>
+      </c>
+      <c r="F21" s="6">
+        <f>MAX(NormMatrix!F21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <f>MAX(NormMatrix!G21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <f>MAX(NormMatrix!H21,0)</f>
+        <v>9.5852757712291584E-2</v>
+      </c>
+      <c r="I21" s="6">
+        <f>MAX(NormMatrix!I21,0)</f>
+        <v>6.9644128532871608E-2</v>
+      </c>
+      <c r="J21" s="6">
+        <f>MAX(NormMatrix!J21,0)</f>
+        <v>0.26172689797317195</v>
+      </c>
+      <c r="K21" s="6">
+        <f>MAX(NormMatrix!K21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <f>MAX(NormMatrix!L21,0)</f>
+        <v>8.1257459091567674E-3</v>
+      </c>
+      <c r="M21" s="6">
+        <f>MAX(NormMatrix!M21,0)</f>
+        <v>0.20034130425780755</v>
+      </c>
+      <c r="N21" s="6">
+        <f>MAX(NormMatrix!N21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
+        <f>MAX(NormMatrix!O21,0)</f>
+        <v>0.18378736966385822</v>
+      </c>
+      <c r="P21" s="6">
+        <f>MAX(NormMatrix!P21,0)</f>
+        <v>0.2737799846803744</v>
+      </c>
+      <c r="Q21" s="6">
+        <f>MAX(NormMatrix!Q21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="6">
+        <f>MAX(NormMatrix!R21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="6">
+        <f>MAX(NormMatrix!S21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="6">
+        <f>MAX(NormMatrix!T21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="6">
+        <f>MAX(NormMatrix!U21,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4">
+        <f>LARGE($B$3:$B$21, 1)</f>
+        <v>0.55444750193353987</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4">
+        <f>LARGE($B$3:$B$21, 2)</f>
+        <v>0.35577972454766577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4">
+        <f>LARGE($B$3:$B$21, 3)</f>
+        <v>0.29501316508704806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4">
+        <f>LARGE($B$3:$B$21, 4)</f>
+        <v>0.21597537370665254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="4">
+        <f>LARGE($B$3:$B$21, 5)</f>
+        <v>0.19279858482944665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:U21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
✨ Item-item CF: complete part 4
</commit_message>
<xml_diff>
--- a/recommender-systems/collaborative-filtering/Assignment 5.xlsx
+++ b/recommender-systems/collaborative-filtering/Assignment 5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eigenein/GitHub/coursera/recommender-systems/collaborative-filtering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB560C1-6EE3-A64C-B47A-B7790D246637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52C1A32-0A3C-D747-AB1C-29CE4C992D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratings" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="30">
   <si>
     <t>User</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>5th top-most</t>
+  </si>
+  <si>
+    <t>Part Ⅳ</t>
   </si>
 </sst>
 </file>
@@ -961,13 +964,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2036,89 +2039,174 @@
         <v>23</v>
       </c>
       <c r="B23" s="9" cm="1">
-        <f t="array" ref="B23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!B2:B21) / SUMPRODUCT(FilterMatrix!B$2:B$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="B23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!B$2:B$21) / SUMPRODUCT(FilterMatrix!B$2:B$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.6668982678575537</v>
       </c>
       <c r="C23" s="9" cm="1">
-        <f t="array" ref="C23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!C2:C21) / SUMPRODUCT(FilterMatrix!C$2:C$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="C23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!C$2:C$21) / SUMPRODUCT(FilterMatrix!C$2:C$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7742152158304081</v>
       </c>
       <c r="D23" s="9" cm="1">
-        <f t="array" ref="D23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!D2:D21) / SUMPRODUCT(FilterMatrix!D$2:D$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="D23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!D$2:D$21) / SUMPRODUCT(FilterMatrix!D$2:D$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7085502730962281</v>
       </c>
       <c r="E23" s="9" cm="1">
-        <f t="array" ref="E23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!E2:E21) / SUMPRODUCT(FilterMatrix!E$2:E$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="E23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!E$2:E$21) / SUMPRODUCT(FilterMatrix!E$2:E$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7239631000194673</v>
       </c>
       <c r="F23" s="9" cm="1">
-        <f t="array" ref="F23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!F2:F21) / SUMPRODUCT(FilterMatrix!F$2:F$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="F23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!F$2:F$21) / SUMPRODUCT(FilterMatrix!F$2:F$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.8833041592722894</v>
       </c>
       <c r="G23" s="9" cm="1">
-        <f t="array" ref="G23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!G2:G21) / SUMPRODUCT(FilterMatrix!G$2:G$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="G23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!G$2:G$21) / SUMPRODUCT(FilterMatrix!G$2:G$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.8097667519781768</v>
       </c>
       <c r="H23" s="9" cm="1">
-        <f t="array" ref="H23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!H2:H21) / SUMPRODUCT(FilterMatrix!H$2:H$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="H23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!H$2:H$21) / SUMPRODUCT(FilterMatrix!H$2:H$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.9222401343343751</v>
       </c>
       <c r="I23" s="9" cm="1">
-        <f t="array" ref="I23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!I2:I21) / SUMPRODUCT(FilterMatrix!I$2:I$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="I23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!I$2:I$21) / SUMPRODUCT(FilterMatrix!I$2:I$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7802181220722759</v>
       </c>
       <c r="J23" s="9" cm="1">
-        <f t="array" ref="J23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!J2:J21) / SUMPRODUCT(FilterMatrix!J$2:J$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="J23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!J$2:J$21) / SUMPRODUCT(FilterMatrix!J$2:J$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.8027971011907153</v>
       </c>
       <c r="K23" s="9" cm="1">
-        <f t="array" ref="K23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!K2:K21) / SUMPRODUCT(FilterMatrix!K$2:K$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="K23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!K$2:K$21) / SUMPRODUCT(FilterMatrix!K$2:K$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.9288008978668989</v>
       </c>
       <c r="L23" s="9" cm="1">
-        <f t="array" ref="L23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!L2:L21) / SUMPRODUCT(FilterMatrix!L$2:L$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="L23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!L$2:L$21) / SUMPRODUCT(FilterMatrix!L$2:L$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.8521305874805973</v>
       </c>
       <c r="M23" s="9" cm="1">
-        <f t="array" ref="M23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!M2:M21) / SUMPRODUCT(FilterMatrix!M$2:M$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="M23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!M$2:M$21) / SUMPRODUCT(FilterMatrix!M$2:M$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7018261412839544</v>
       </c>
       <c r="N23" s="9" cm="1">
-        <f t="array" ref="N23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!N2:N21) / SUMPRODUCT(FilterMatrix!N$2:N$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="N23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!N$2:N$21) / SUMPRODUCT(FilterMatrix!N$2:N$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.674950999537169</v>
       </c>
       <c r="O23" s="9" cm="1">
-        <f t="array" ref="O23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!O2:O21) / SUMPRODUCT(FilterMatrix!O$2:O$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="O23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!O$2:O$21) / SUMPRODUCT(FilterMatrix!O$2:O$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7842520940793496</v>
       </c>
       <c r="P23" s="9" cm="1">
-        <f t="array" ref="P23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!P2:P21) / SUMPRODUCT(FilterMatrix!P$2:P$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="P23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!P$2:P$21) / SUMPRODUCT(FilterMatrix!P$2:P$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.6907197332431223</v>
       </c>
       <c r="Q23" s="9" cm="1">
-        <f t="array" ref="Q23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!Q2:Q21) / SUMPRODUCT(FilterMatrix!Q$2:Q$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="Q23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!Q$2:Q$21) / SUMPRODUCT(FilterMatrix!Q$2:Q$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7701762031234276</v>
       </c>
       <c r="R23" s="9" cm="1">
-        <f t="array" ref="R23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!R2:R21) / SUMPRODUCT(FilterMatrix!R$2:R$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="R23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!R$2:R$21) / SUMPRODUCT(FilterMatrix!R$2:R$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.9738833825830233</v>
       </c>
       <c r="S23" s="9" cm="1">
-        <f t="array" ref="S23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!S2:S21) / SUMPRODUCT(FilterMatrix!S$2:S$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="S23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!S$2:S$21) / SUMPRODUCT(FilterMatrix!S$2:S$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.7162671331726407</v>
       </c>
       <c r="T23" s="9" cm="1">
-        <f t="array" ref="T23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!T2:T21) / SUMPRODUCT(FilterMatrix!T$2:T$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="T23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!T$2:T$21) / SUMPRODUCT(FilterMatrix!T$2:T$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.8181547746216626</v>
       </c>
       <c r="U23" s="9" cm="1">
-        <f t="array" ref="U23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!U2:U21) / SUMPRODUCT(FilterMatrix!U$2:U$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <f t="array" ref="U23">SUMPRODUCT(TRANSPOSE($B$3:$U$3), FilterMatrix!U$2:U$21) / SUMPRODUCT(FilterMatrix!U$2:U$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
         <v>2.6109454185869558</v>
       </c>
     </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="9" cm="1">
+        <f t="array" ref="B24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!B$2:B$21) / SUMPRODUCT(NormFilterMatrix!B$2:B$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>1.4668511909374318</v>
+      </c>
+      <c r="C24" s="9" cm="1">
+        <f t="array" ref="C24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!C$2:C$21) / SUMPRODUCT(NormFilterMatrix!C$2:C$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.7896174628909431</v>
+      </c>
+      <c r="D24" s="9" cm="1">
+        <f t="array" ref="D24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!D$2:D$21) / SUMPRODUCT(NormFilterMatrix!D$2:D$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.9044717440264747</v>
+      </c>
+      <c r="E24" s="9" cm="1">
+        <f t="array" ref="E24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!E$2:E$21) / SUMPRODUCT(NormFilterMatrix!E$2:E$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>1.8401363249643843</v>
+      </c>
+      <c r="F24" s="9" cm="1">
+        <f t="array" ref="F24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!F$2:F$21) / SUMPRODUCT(NormFilterMatrix!F$2:F$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>3.2208901152339235</v>
+      </c>
+      <c r="G24" s="9" cm="1">
+        <f t="array" ref="G24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!G$2:G$21) / SUMPRODUCT(NormFilterMatrix!G$2:G$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.3240261956539787</v>
+      </c>
+      <c r="H24" s="9" cm="1">
+        <f t="array" ref="H24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!H$2:H$21) / SUMPRODUCT(NormFilterMatrix!H$2:H$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>4.5658217726160029</v>
+      </c>
+      <c r="I24" s="9" cm="1">
+        <f t="array" ref="I24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!I$2:I$21) / SUMPRODUCT(NormFilterMatrix!I$2:I$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>3.0959173304650731</v>
+      </c>
+      <c r="J24" s="9" cm="1">
+        <f t="array" ref="J24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!J$2:J$21) / SUMPRODUCT(NormFilterMatrix!J$2:J$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.8044268597807345</v>
+      </c>
+      <c r="K24" s="9" cm="1">
+        <f t="array" ref="K24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!K$2:K$21) / SUMPRODUCT(NormFilterMatrix!K$2:K$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>3.6021413989484481</v>
+      </c>
+      <c r="L24" s="9" cm="1">
+        <f t="array" ref="L24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!L$2:L$21) / SUMPRODUCT(NormFilterMatrix!L$2:L$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>3.2979383133590172</v>
+      </c>
+      <c r="M24" s="9" cm="1">
+        <f t="array" ref="M24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!M$2:M$21) / SUMPRODUCT(NormFilterMatrix!M$2:M$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>1.9961937149814069</v>
+      </c>
+      <c r="N24" s="9" cm="1">
+        <f t="array" ref="N24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!N$2:N$21) / SUMPRODUCT(NormFilterMatrix!N$2:N$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.0431634599946387</v>
+      </c>
+      <c r="O24" s="9" cm="1">
+        <f t="array" ref="O24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!O$2:O$21) / SUMPRODUCT(NormFilterMatrix!O$2:O$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.6416328106688471</v>
+      </c>
+      <c r="P24" s="9" cm="1">
+        <f t="array" ref="P24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!P$2:P$21) / SUMPRODUCT(NormFilterMatrix!P$2:P$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>1.9228172151677461</v>
+      </c>
+      <c r="Q24" s="9" cm="1">
+        <f t="array" ref="Q24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!Q$2:Q$21) / SUMPRODUCT(NormFilterMatrix!Q$2:Q$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.6812038229452591</v>
+      </c>
+      <c r="R24" s="9" cm="1">
+        <f t="array" ref="R24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!R$2:R$21) / SUMPRODUCT(NormFilterMatrix!R$2:R$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>4.562482819188924</v>
+      </c>
+      <c r="S24" s="9" cm="1">
+        <f t="array" ref="S24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!S$2:S$21) / SUMPRODUCT(NormFilterMatrix!S$2:S$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.0327368468284646</v>
+      </c>
+      <c r="T24" s="9" cm="1">
+        <f t="array" ref="T24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!T$2:T$21) / SUMPRODUCT(NormFilterMatrix!T$2:T$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>2.861378038375844</v>
+      </c>
+      <c r="U24" s="9" cm="1">
+        <f t="array" ref="U24">SUMPRODUCT(TRANSPOSE($B$3:$U$3), NormFilterMatrix!U$2:U$21) / SUMPRODUCT(NormFilterMatrix!U$2:U$21, TRANSPOSE(SIGN($B$3:$U$3)))</f>
+        <v>1.8222875550508626</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B23:U23">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B23:U24">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9640,7 +9728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CE2943-F9C7-2D4E-B536-8569BAE68B47}">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>